<commit_message>
Complete Add Grants Form
Add Grants Form is now able to save. What is pending is the editing.
</commit_message>
<xml_diff>
--- a/web/database_design.xlsx
+++ b/web/database_design.xlsx
@@ -9,34 +9,35 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15210" windowHeight="6240" tabRatio="957"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15210" windowHeight="6240" tabRatio="957" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="grants_infor" sheetId="1" r:id="rId1"/>
-    <sheet name="solicitation_infor" sheetId="41" r:id="rId2"/>
-    <sheet name="opts_submissionmeans" sheetId="42" r:id="rId3"/>
-    <sheet name="applicants_details" sheetId="49" r:id="rId4"/>
-    <sheet name="evaluation_details" sheetId="54" r:id="rId5"/>
-    <sheet name="pre_award_assessment" sheetId="50" r:id="rId6"/>
-    <sheet name="opts_recommendation" sheetId="52" r:id="rId7"/>
-    <sheet name="opts_modification_number" sheetId="53" r:id="rId8"/>
-    <sheet name="subrecipient_infor" sheetId="6" r:id="rId9"/>
-    <sheet name="opts_subrecipientstatus" sheetId="44" r:id="rId10"/>
-    <sheet name="opts_subaward_type" sheetId="11" r:id="rId11"/>
-    <sheet name="opts_applicable_indirect_cost" sheetId="10" r:id="rId12"/>
-    <sheet name="opts_entitytype" sheetId="9" r:id="rId13"/>
-    <sheet name="opts_reportingfrequency" sheetId="8" r:id="rId14"/>
-    <sheet name="opts_currency" sheetId="7" r:id="rId15"/>
-    <sheet name="subaward_lop_budget" sheetId="12" r:id="rId16"/>
-    <sheet name="obligation_infor" sheetId="17" r:id="rId17"/>
-    <sheet name="modification_details" sheetId="22" r:id="rId18"/>
-    <sheet name="financial_reports" sheetId="30" r:id="rId19"/>
-    <sheet name="cost_share_infor" sheetId="35" r:id="rId20"/>
-    <sheet name="sub_award_close_out" sheetId="51" r:id="rId21"/>
+    <sheet name="key input fields" sheetId="55" r:id="rId1"/>
+    <sheet name="grants_infor" sheetId="1" r:id="rId2"/>
+    <sheet name="solicitation_infor" sheetId="41" r:id="rId3"/>
+    <sheet name="opts_submissionmeans" sheetId="42" r:id="rId4"/>
+    <sheet name="applicants_details" sheetId="49" r:id="rId5"/>
+    <sheet name="evaluation_details" sheetId="54" r:id="rId6"/>
+    <sheet name="pre_award_assessment" sheetId="50" r:id="rId7"/>
+    <sheet name="opts_recommendation" sheetId="52" r:id="rId8"/>
+    <sheet name="opts_modification_number" sheetId="53" r:id="rId9"/>
+    <sheet name="subrecipient_infor" sheetId="6" r:id="rId10"/>
+    <sheet name="opts_subrecipientstatus" sheetId="44" r:id="rId11"/>
+    <sheet name="opts_subaward_type" sheetId="11" r:id="rId12"/>
+    <sheet name="opts_applicable_indirect_cost" sheetId="10" r:id="rId13"/>
+    <sheet name="opts_entitytype" sheetId="9" r:id="rId14"/>
+    <sheet name="opts_reportingfrequency" sheetId="8" r:id="rId15"/>
+    <sheet name="opts_currency" sheetId="7" r:id="rId16"/>
+    <sheet name="subaward_lop_budget" sheetId="12" r:id="rId17"/>
+    <sheet name="obligation_infor" sheetId="17" r:id="rId18"/>
+    <sheet name="modification_details" sheetId="22" r:id="rId19"/>
+    <sheet name="financial_reports" sheetId="30" r:id="rId20"/>
+    <sheet name="cost_share_infor" sheetId="35" r:id="rId21"/>
+    <sheet name="sub_award_close_out" sheetId="51" r:id="rId22"/>
   </sheets>
   <definedNames>
-    <definedName name="_Hlk100664909" localSheetId="0">grants_infor!$F$7</definedName>
-    <definedName name="OLE_LINK1" localSheetId="8">subrecipient_infor!$A$10</definedName>
+    <definedName name="_Hlk100664909" localSheetId="1">grants_infor!$F$7</definedName>
+    <definedName name="OLE_LINK1" localSheetId="9">subrecipient_infor!$A$10</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -48,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="821" uniqueCount="583">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="873" uniqueCount="605">
   <si>
     <t>1.0 Grant Information</t>
   </si>
@@ -2893,9 +2894,6 @@
     </r>
   </si>
   <si>
-    <t>Get the donor_code</t>
-  </si>
-  <si>
     <t>This carries</t>
   </si>
   <si>
@@ -3015,9 +3013,6 @@
     <t>Award_amount</t>
   </si>
   <si>
-    <t>award_amount</t>
-  </si>
-  <si>
     <t>subaward_agreement_location</t>
   </si>
   <si>
@@ -4980,9 +4975,6 @@
     <t>sdhgfddsjs</t>
   </si>
   <si>
-    <t>This data should be saved on the applicant details tables. On the interface, it will require a new</t>
-  </si>
-  <si>
     <t>sub_recipient_id</t>
   </si>
   <si>
@@ -5023,6 +5015,95 @@
   </si>
   <si>
     <t>sdfsfdsfswerw</t>
+  </si>
+  <si>
+    <t>This data should be saved on the applicant details tables. On the interface, it will require a new one</t>
+  </si>
+  <si>
+    <t>Donor Name</t>
+  </si>
+  <si>
+    <t>Donar Code</t>
+  </si>
+  <si>
+    <t>Prime Recipient</t>
+  </si>
+  <si>
+    <t>Prime Award Number</t>
+  </si>
+  <si>
+    <t>Country of Implementation</t>
+  </si>
+  <si>
+    <t>Implementation Start Date</t>
+  </si>
+  <si>
+    <t>Implemntation End Date</t>
+  </si>
+  <si>
+    <t>Obligation End Date</t>
+  </si>
+  <si>
+    <t>Cost Share Obligation</t>
+  </si>
+  <si>
+    <t>Grant Amount</t>
+  </si>
+  <si>
+    <t>input Field</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>input</t>
+  </si>
+  <si>
+    <t>select</t>
+  </si>
+  <si>
+    <t>input date</t>
+  </si>
+  <si>
+    <t>Teaxt Area</t>
+  </si>
+  <si>
+    <t>Select</t>
+  </si>
+  <si>
+    <t>Input</t>
+  </si>
+  <si>
+    <t>Input with placeholder</t>
+  </si>
+  <si>
+    <t>&lt;div class='form-group'&gt;
+&lt;label for='exampleInputEmail1'&gt;Email address&lt;/label&gt;
+&lt;input type='input' class='form-control' id='exampleInputEmail1' name=''  placeholder=''/&gt;
+&lt;/div&gt;</t>
+  </si>
+  <si>
+    <t>&lt;div class='form-group'&gt;
+&lt;label for='exampleInputEmail1'&gt;Email address&lt;/label&gt;
+&lt;input type='input' class='form-control' id='exampleInputEmail1' aria-describedby='emailHelp' name=''  placeholder=''&gt;
+&lt;small id='emailHelp' class='form-text text-muted'&gt;We'll never share your email with anyone else.&lt;/small&gt;
+&lt;/div&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> &lt;div class='form-group'&gt;
+&lt;label for='exampleFormControlTextarea1'&gt;Example textarea&lt;/label&gt;
+&lt;textarea class='form-control' id='exampleFormControlTextarea1' rows='3'&gt;&lt;/textarea&gt;
+&lt;/div&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> &lt;div class='form-group'&gt;
+&lt;label for='exampleFormControlSelect1'&gt;Example select&lt;/label&gt;
+&lt;select class='form-control' id='exampleFormControlSelect1'&gt;
+&lt;/select&gt;
+&lt;/div&gt;</t>
+  </si>
+  <si>
+    <t>Deloitte &amp; Touche Limited</t>
   </si>
 </sst>
 </file>
@@ -5116,7 +5197,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="15">
+  <borders count="16">
     <border>
       <left/>
       <right/>
@@ -5286,11 +5367,24 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="77">
+  <cellXfs count="83">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="4"/>
@@ -5404,21 +5498,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
@@ -5429,6 +5508,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -5455,6 +5540,33 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -5736,162 +5848,313 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr codeName="Sheet1">
-    <tabColor theme="4"/>
-  </sheetPr>
-  <dimension ref="A1:L18"/>
+  <dimension ref="B6:C14"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="8.265625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="39" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.59765625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.59765625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="21" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="67.86328125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="24.86328125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="24.265625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="18.73046875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="19.73046875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.59765625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="34.9296875" style="81" customWidth="1"/>
+    <col min="3" max="3" width="107.06640625" customWidth="1"/>
+    <col min="4" max="4" width="43.1328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A1" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="I1" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="J1" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="K1" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="L1" s="27" t="s">
-        <v>381</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A2" s="4">
-        <v>1</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>416</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="E2" s="4">
-        <v>84478</v>
-      </c>
-      <c r="F2" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="G2" s="5">
-        <v>44317</v>
-      </c>
-      <c r="H2" s="5">
-        <v>46142</v>
-      </c>
-      <c r="I2" s="5">
-        <v>46142</v>
-      </c>
-      <c r="J2" s="3"/>
-      <c r="K2" s="3"/>
-      <c r="L2" s="3"/>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="F6" s="2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="F7" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="F8" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="F9" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="F10" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="F11" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="F12" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="F13" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="F14" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="F15" s="1" t="s">
-        <v>380</v>
-      </c>
-    </row>
-    <row r="18" spans="4:4" x14ac:dyDescent="0.45">
-      <c r="D18" s="6" t="s">
-        <v>361</v>
+    <row r="6" spans="2:3" ht="71.25" x14ac:dyDescent="0.45">
+      <c r="B6" s="82" t="s">
+        <v>596</v>
+      </c>
+      <c r="C6" s="80" t="s">
+        <v>602</v>
+      </c>
+    </row>
+    <row r="8" spans="2:3" ht="71.25" x14ac:dyDescent="0.45">
+      <c r="B8" s="82" t="s">
+        <v>597</v>
+      </c>
+      <c r="C8" s="80" t="s">
+        <v>603</v>
+      </c>
+    </row>
+    <row r="11" spans="2:3" ht="85.5" x14ac:dyDescent="0.45">
+      <c r="B11" s="82" t="s">
+        <v>598</v>
+      </c>
+      <c r="C11" s="80" t="s">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="14" spans="2:3" ht="71.25" x14ac:dyDescent="0.45">
+      <c r="B14" s="82" t="s">
+        <v>599</v>
+      </c>
+      <c r="C14" s="80" t="s">
+        <v>601</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet2">
+    <tabColor theme="4"/>
+  </sheetPr>
+  <dimension ref="A1:S18"/>
+  <sheetViews>
+    <sheetView showGridLines="0" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="32.1328125" customWidth="1"/>
+    <col min="2" max="2" width="15" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.86328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.1328125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.73046875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.86328125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.265625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.59765625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="26" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="30.3984375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.59765625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="17.73046875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="17.3984375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="19.73046875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="30" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="21.59765625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:19" x14ac:dyDescent="0.45">
+      <c r="A1" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="D1" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="E1" s="9" t="s">
+        <v>231</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="H1" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="I1" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="J1" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="K1" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="L1" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="M1" s="9" t="s">
+        <v>232</v>
+      </c>
+      <c r="N1" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="O1" s="23" t="s">
+        <v>381</v>
+      </c>
+      <c r="P1" s="23" t="s">
+        <v>380</v>
+      </c>
+      <c r="Q1" s="23" t="s">
+        <v>382</v>
+      </c>
+      <c r="R1" s="23" t="s">
+        <v>383</v>
+      </c>
+      <c r="S1" s="24" t="s">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.45">
+      <c r="A2" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>226</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>227</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>233</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>247</v>
+      </c>
+      <c r="F2" s="5">
+        <v>44564</v>
+      </c>
+      <c r="G2" s="5">
+        <v>46111</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>241</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>219</v>
+      </c>
+      <c r="K2" s="3" t="s">
+        <v>243</v>
+      </c>
+      <c r="L2" s="3" t="s">
+        <v>215</v>
+      </c>
+      <c r="M2" s="3" t="s">
+        <v>246</v>
+      </c>
+      <c r="N2" s="3" t="s">
+        <v>245</v>
+      </c>
+      <c r="O2" s="23" t="s">
+        <v>329</v>
+      </c>
+      <c r="P2" s="23" t="s">
+        <v>330</v>
+      </c>
+      <c r="Q2" s="23" t="s">
+        <v>329</v>
+      </c>
+      <c r="R2" s="23" t="s">
+        <v>330</v>
+      </c>
+      <c r="S2" s="24" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.45">
+      <c r="D3" t="s">
+        <v>238</v>
+      </c>
+      <c r="H3" t="s">
+        <v>239</v>
+      </c>
+      <c r="I3" t="s">
+        <v>240</v>
+      </c>
+      <c r="J3" t="s">
+        <v>242</v>
+      </c>
+      <c r="L3" t="s">
+        <v>244</v>
+      </c>
+      <c r="S3" s="25" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.45">
+      <c r="S4" s="25" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" ht="60" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B6" s="74" t="s">
+        <v>388</v>
+      </c>
+      <c r="C6" s="74"/>
+      <c r="D6" s="74"/>
+      <c r="E6" s="74"/>
+      <c r="F6" s="74"/>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.45">
+      <c r="A8" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.45">
+      <c r="A9" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.45">
+      <c r="A10" s="7" t="s">
+        <v>366</v>
+      </c>
+      <c r="B10" s="6"/>
+      <c r="C10" s="6"/>
+      <c r="D10" s="6"/>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.45">
+      <c r="A11" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.45">
+      <c r="A12" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.45">
+      <c r="A13" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="B13" s="6"/>
+      <c r="C13" s="6"/>
+    </row>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.45">
+      <c r="A14" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="B14" s="6"/>
+      <c r="C14" s="6"/>
+    </row>
+    <row r="15" spans="1:19" x14ac:dyDescent="0.45">
+      <c r="A15" s="7" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="16" spans="1:19" x14ac:dyDescent="0.45">
+      <c r="A16" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A17" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="B17" s="6"/>
+      <c r="C17" s="6"/>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A18" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C18" t="s">
+        <v>376</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B6:F6"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet16">
     <tabColor theme="4"/>
@@ -5913,18 +6176,18 @@
         <v>9</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A2" s="3" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="C2" s="3">
         <v>1</v>
@@ -5932,10 +6195,10 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A3" s="3" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="C3" s="3">
         <v>1</v>
@@ -5943,10 +6206,10 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A4" s="3" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="C4" s="3">
         <v>1</v>
@@ -5957,7 +6220,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet3">
     <tabColor theme="4"/>
@@ -5982,7 +6245,7 @@
         <v>236</v>
       </c>
       <c r="C1" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.45">
@@ -6034,7 +6297,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet4">
     <tabColor theme="4"/>
@@ -6059,7 +6322,7 @@
         <v>218</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.45">
@@ -6105,7 +6368,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet5">
     <tabColor theme="4"/>
@@ -6129,7 +6392,7 @@
         <v>237</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.45">
@@ -6214,7 +6477,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet6">
     <tabColor theme="4"/>
@@ -6238,7 +6501,7 @@
         <v>36</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.45">
@@ -6290,7 +6553,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet7">
     <tabColor theme="4"/>
@@ -6315,7 +6578,7 @@
         <v>45</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.45">
@@ -7234,7 +7497,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet8">
     <tabColor theme="4"/>
@@ -7283,7 +7546,7 @@
         <v>261</v>
       </c>
       <c r="G1" s="23" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="H1" s="3" t="s">
         <v>262</v>
@@ -7313,7 +7576,7 @@
         <v>271</v>
       </c>
       <c r="Q1" s="22" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
     </row>
     <row r="2" spans="1:17" ht="142.5" x14ac:dyDescent="0.45">
@@ -7336,7 +7599,7 @@
         <v>278</v>
       </c>
       <c r="G2" s="23" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="H2" s="3" t="s">
         <v>277</v>
@@ -7366,7 +7629,7 @@
         <v>1</v>
       </c>
       <c r="Q2" s="26" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.45">
@@ -7376,7 +7639,7 @@
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.45">
       <c r="D7" s="11" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.45">
@@ -7429,7 +7692,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet9">
     <tabColor theme="8"/>
@@ -7477,7 +7740,7 @@
         <v>259</v>
       </c>
       <c r="F1" s="23" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="G1" s="3" t="s">
         <v>260</v>
@@ -7531,7 +7794,7 @@
         <v>280</v>
       </c>
       <c r="F2" s="23" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="G2" s="3" t="s">
         <v>279</v>
@@ -7631,7 +7894,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet10">
     <tabColor theme="4"/>
@@ -7689,7 +7952,7 @@
         <v>33</v>
       </c>
       <c r="C1" s="29" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="D1" s="29" t="s">
         <v>302</v>
@@ -7707,31 +7970,31 @@
         <v>305</v>
       </c>
       <c r="I1" s="30" t="s">
+        <v>392</v>
+      </c>
+      <c r="J1" s="30" t="s">
+        <v>393</v>
+      </c>
+      <c r="K1" s="30" t="s">
         <v>394</v>
       </c>
-      <c r="J1" s="30" t="s">
+      <c r="L1" s="30" t="s">
         <v>395</v>
       </c>
-      <c r="K1" s="30" t="s">
+      <c r="M1" s="30" t="s">
         <v>396</v>
       </c>
-      <c r="L1" s="30" t="s">
+      <c r="N1" s="30" t="s">
         <v>397</v>
       </c>
-      <c r="M1" s="30" t="s">
+      <c r="O1" s="30" t="s">
         <v>398</v>
       </c>
-      <c r="N1" s="30" t="s">
-        <v>399</v>
-      </c>
-      <c r="O1" s="30" t="s">
-        <v>400</v>
-      </c>
       <c r="P1" s="31" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="Q1" s="31" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="R1" s="29" t="s">
         <v>268</v>
@@ -7748,19 +8011,19 @@
     </row>
     <row r="2" spans="1:37" x14ac:dyDescent="0.45">
       <c r="A2" s="29" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="B2" s="29" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="C2" s="32" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="D2" s="29" t="s">
         <v>259</v>
       </c>
       <c r="E2" s="31" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="F2" s="29" t="s">
         <v>260</v>
@@ -7781,22 +8044,22 @@
         <v>318</v>
       </c>
       <c r="L2" s="29" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="M2" s="29" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="N2" s="29" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="O2" s="29" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="P2" s="29" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="Q2" s="29" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="R2" s="14">
         <v>44965.416701388887</v>
@@ -7805,13 +8068,13 @@
         <v>44965.416701388887</v>
       </c>
       <c r="T2" s="29" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="U2" s="29">
         <v>1</v>
       </c>
       <c r="AA2" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="AF2" s="23" t="s">
         <v>329</v>
@@ -7837,22 +8100,22 @@
     </row>
     <row r="4" spans="1:37" x14ac:dyDescent="0.45">
       <c r="C4" s="3" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
     </row>
     <row r="5" spans="1:37" x14ac:dyDescent="0.45">
       <c r="C5" s="3" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
     </row>
     <row r="6" spans="1:37" x14ac:dyDescent="0.45">
       <c r="C6" s="3" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
     </row>
     <row r="7" spans="1:37" x14ac:dyDescent="0.45">
       <c r="C7" s="3" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="G7" s="15" t="s">
         <v>296</v>
@@ -7880,7 +8143,7 @@
     </row>
     <row r="11" spans="1:37" x14ac:dyDescent="0.45">
       <c r="D11" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="G11" s="18" t="s">
         <v>300</v>
@@ -7888,7 +8151,7 @@
     </row>
     <row r="12" spans="1:37" x14ac:dyDescent="0.45">
       <c r="D12" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="G12" s="18" t="s">
         <v>301</v>
@@ -7899,17 +8162,17 @@
     </row>
     <row r="13" spans="1:37" x14ac:dyDescent="0.45">
       <c r="G13" s="23" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
     </row>
     <row r="14" spans="1:37" x14ac:dyDescent="0.45">
       <c r="G14" s="23" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
     </row>
     <row r="15" spans="1:37" x14ac:dyDescent="0.45">
       <c r="G15" s="23" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
     </row>
     <row r="16" spans="1:37" x14ac:dyDescent="0.45">
@@ -7917,22 +8180,22 @@
         <v>308</v>
       </c>
       <c r="G16" s="23" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
     </row>
     <row r="17" spans="7:7" x14ac:dyDescent="0.45">
       <c r="G17" s="23" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
     </row>
     <row r="18" spans="7:7" x14ac:dyDescent="0.45">
       <c r="G18" s="23" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
     </row>
     <row r="19" spans="7:7" x14ac:dyDescent="0.45">
       <c r="G19" s="23" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
     </row>
   </sheetData>
@@ -7941,7 +8204,412 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet1">
+    <tabColor theme="4"/>
+  </sheetPr>
+  <dimension ref="A1:K26"/>
+  <sheetViews>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="E25" sqref="E25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="23" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="39" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.265625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.59765625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="73.73046875" customWidth="1"/>
+    <col min="6" max="6" width="67.86328125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="24.86328125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="24.265625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18.73046875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="19.73046875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.59765625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A1" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A2" s="4">
+        <v>1</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>414</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>604</v>
+      </c>
+      <c r="E2" s="4">
+        <v>84478</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="G2" s="5">
+        <v>44317</v>
+      </c>
+      <c r="H2" s="5">
+        <v>46142</v>
+      </c>
+      <c r="I2" s="5">
+        <v>46142</v>
+      </c>
+      <c r="J2" s="3"/>
+      <c r="K2" s="3"/>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="B3" t="s">
+        <v>581</v>
+      </c>
+      <c r="C3" t="s">
+        <v>582</v>
+      </c>
+      <c r="D3" t="s">
+        <v>583</v>
+      </c>
+      <c r="E3" t="s">
+        <v>584</v>
+      </c>
+      <c r="F3" t="s">
+        <v>585</v>
+      </c>
+      <c r="G3" t="s">
+        <v>586</v>
+      </c>
+      <c r="H3" t="s">
+        <v>587</v>
+      </c>
+      <c r="I3" t="s">
+        <v>588</v>
+      </c>
+      <c r="J3" t="s">
+        <v>589</v>
+      </c>
+      <c r="K3" t="s">
+        <v>590</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="F6" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="F7" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="F8" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="F9" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="F10" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="F11" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="F12" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="F13" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="F14" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="F15" s="1" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A16" s="39" t="s">
+        <v>9</v>
+      </c>
+      <c r="B16" s="39"/>
+      <c r="C16" s="39" t="s">
+        <v>591</v>
+      </c>
+      <c r="D16" s="39" t="s">
+        <v>592</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="59.65" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A17" s="77" t="s">
+        <v>11</v>
+      </c>
+      <c r="B17" s="78" t="s">
+        <v>414</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>581</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>593</v>
+      </c>
+      <c r="E17" s="80" t="str">
+        <f>"&lt;div class='form-group col-md-4'&gt;
+&lt;label for='"&amp;A17&amp;"'&gt;&lt;b&gt;"&amp;C17&amp;"&lt;font color='red'&gt;*&lt;/font&gt;&lt;/b&gt;&lt;/label&gt;
+&lt;input type='input' class='form-control' id='"&amp;A17&amp;"' name='"&amp;A17&amp;"'  placeholder='Enter "&amp;C17&amp;"'/&gt;
+&lt;/div&gt;"</f>
+        <v>&lt;div class='form-group col-md-4'&gt;
+&lt;label for='donor_name'&gt;&lt;b&gt;Donor Name&lt;font color='red'&gt;*&lt;/font&gt;&lt;/b&gt;&lt;/label&gt;
+&lt;input type='input' class='form-control' id='donor_name' name='donor_name'  placeholder='Enter Donor Name'/&gt;
+&lt;/div&gt;</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="61.15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A18" s="77" t="s">
+        <v>22</v>
+      </c>
+      <c r="B18" s="78" t="s">
+        <v>17</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>582</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>593</v>
+      </c>
+      <c r="E18" s="80" t="str">
+        <f t="shared" ref="E18:E25" si="0">"&lt;div class='form-group col-md-4'&gt;
+&lt;label for='"&amp;A18&amp;"'&gt;&lt;b&gt;"&amp;C18&amp;"&lt;font color='red'&gt;*&lt;/font&gt;&lt;/b&gt;&lt;/label&gt;
+&lt;input type='input' class='form-control' id='"&amp;A18&amp;"' name='"&amp;A18&amp;"'  placeholder='Enter "&amp;C18&amp;"'/&gt;
+&lt;/div&gt;"</f>
+        <v>&lt;div class='form-group col-md-4'&gt;
+&lt;label for='donor_code'&gt;&lt;b&gt;Donar Code&lt;font color='red'&gt;*&lt;/font&gt;&lt;/b&gt;&lt;/label&gt;
+&lt;input type='input' class='form-control' id='donor_code' name='donor_code'  placeholder='Enter Donar Code'/&gt;
+&lt;/div&gt;</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="71.25" x14ac:dyDescent="0.45">
+      <c r="A19" s="77" t="s">
+        <v>12</v>
+      </c>
+      <c r="B19" s="78" t="s">
+        <v>18</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>583</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>593</v>
+      </c>
+      <c r="E19" s="80" t="str">
+        <f t="shared" si="0"/>
+        <v>&lt;div class='form-group col-md-4'&gt;
+&lt;label for='prime_recipient'&gt;&lt;b&gt;Prime Recipient&lt;font color='red'&gt;*&lt;/font&gt;&lt;/b&gt;&lt;/label&gt;
+&lt;input type='input' class='form-control' id='prime_recipient' name='prime_recipient'  placeholder='Enter Prime Recipient'/&gt;
+&lt;/div&gt;</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="71.25" x14ac:dyDescent="0.45">
+      <c r="A20" s="77" t="s">
+        <v>13</v>
+      </c>
+      <c r="B20" s="78">
+        <v>84478</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>584</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>593</v>
+      </c>
+      <c r="E20" s="80" t="str">
+        <f t="shared" si="0"/>
+        <v>&lt;div class='form-group col-md-4'&gt;
+&lt;label for='prime_award_number'&gt;&lt;b&gt;Prime Award Number&lt;font color='red'&gt;*&lt;/font&gt;&lt;/b&gt;&lt;/label&gt;
+&lt;input type='input' class='form-control' id='prime_award_number' name='prime_award_number'  placeholder='Enter Prime Award Number'/&gt;
+&lt;/div&gt;</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="71.25" x14ac:dyDescent="0.45">
+      <c r="A21" s="77" t="s">
+        <v>14</v>
+      </c>
+      <c r="B21" s="78" t="s">
+        <v>21</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>585</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>594</v>
+      </c>
+      <c r="E21" s="80" t="str">
+        <f t="shared" si="0"/>
+        <v>&lt;div class='form-group col-md-4'&gt;
+&lt;label for='country_of_implementation'&gt;&lt;b&gt;Country of Implementation&lt;font color='red'&gt;*&lt;/font&gt;&lt;/b&gt;&lt;/label&gt;
+&lt;input type='input' class='form-control' id='country_of_implementation' name='country_of_implementation'  placeholder='Enter Country of Implementation'/&gt;
+&lt;/div&gt;</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="71.25" x14ac:dyDescent="0.45">
+      <c r="A22" s="77" t="s">
+        <v>19</v>
+      </c>
+      <c r="B22" s="79">
+        <v>44317</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>586</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>595</v>
+      </c>
+      <c r="E22" s="80" t="str">
+        <f t="shared" si="0"/>
+        <v>&lt;div class='form-group col-md-4'&gt;
+&lt;label for='implementation_startdate'&gt;&lt;b&gt;Implementation Start Date&lt;font color='red'&gt;*&lt;/font&gt;&lt;/b&gt;&lt;/label&gt;
+&lt;input type='input' class='form-control' id='implementation_startdate' name='implementation_startdate'  placeholder='Enter Implementation Start Date'/&gt;
+&lt;/div&gt;</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="71.25" x14ac:dyDescent="0.45">
+      <c r="A23" s="77" t="s">
+        <v>20</v>
+      </c>
+      <c r="B23" s="79">
+        <v>46142</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>587</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>595</v>
+      </c>
+      <c r="E23" s="80" t="str">
+        <f t="shared" si="0"/>
+        <v>&lt;div class='form-group col-md-4'&gt;
+&lt;label for='implementation_enddate'&gt;&lt;b&gt;Implemntation End Date&lt;font color='red'&gt;*&lt;/font&gt;&lt;/b&gt;&lt;/label&gt;
+&lt;input type='input' class='form-control' id='implementation_enddate' name='implementation_enddate'  placeholder='Enter Implemntation End Date'/&gt;
+&lt;/div&gt;</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="71.25" x14ac:dyDescent="0.45">
+      <c r="A24" s="77" t="s">
+        <v>15</v>
+      </c>
+      <c r="B24" s="79">
+        <v>46142</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>588</v>
+      </c>
+      <c r="D24" s="3" t="s">
+        <v>593</v>
+      </c>
+      <c r="E24" s="80" t="str">
+        <f t="shared" si="0"/>
+        <v>&lt;div class='form-group col-md-4'&gt;
+&lt;label for='obligation_enddate'&gt;&lt;b&gt;Obligation End Date&lt;font color='red'&gt;*&lt;/font&gt;&lt;/b&gt;&lt;/label&gt;
+&lt;input type='input' class='form-control' id='obligation_enddate' name='obligation_enddate'  placeholder='Enter Obligation End Date'/&gt;
+&lt;/div&gt;</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" ht="71.25" x14ac:dyDescent="0.45">
+      <c r="A25" s="77" t="s">
+        <v>16</v>
+      </c>
+      <c r="B25" s="78"/>
+      <c r="C25" s="3" t="s">
+        <v>589</v>
+      </c>
+      <c r="D25" s="3" t="s">
+        <v>593</v>
+      </c>
+      <c r="E25" s="80" t="str">
+        <f t="shared" si="0"/>
+        <v>&lt;div class='form-group col-md-4'&gt;
+&lt;label for='costshare_obligation'&gt;&lt;b&gt;Cost Share Obligation&lt;font color='red'&gt;*&lt;/font&gt;&lt;/b&gt;&lt;/label&gt;
+&lt;input type='input' class='form-control' id='costshare_obligation' name='costshare_obligation'  placeholder='Enter Cost Share Obligation'/&gt;
+&lt;/div&gt;</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" ht="71.25" x14ac:dyDescent="0.45">
+      <c r="A26" s="77" t="s">
+        <v>23</v>
+      </c>
+      <c r="B26" s="78"/>
+      <c r="C26" s="3" t="s">
+        <v>590</v>
+      </c>
+      <c r="D26" s="3"/>
+      <c r="E26" s="80" t="str">
+        <f>"&lt;div class='form-group col-md-4'&gt;
+&lt;label for='"&amp;A26&amp;"'&gt;&lt;b&gt;"&amp;C26&amp;"&lt;font color='red'&gt;*&lt;/font&gt;&lt;/b&gt;&lt;/label&gt;
+&lt;input onkeypress='return numbers(event);'  type='input' class='form-control' id='"&amp;A26&amp;"' name='"&amp;A26&amp;"'  placeholder='Enter "&amp;C26&amp;"'/&gt;
+&lt;/div&gt;"</f>
+        <v>&lt;div class='form-group col-md-4'&gt;
+&lt;label for='grant_amount'&gt;&lt;b&gt;Grant Amount&lt;font color='red'&gt;*&lt;/font&gt;&lt;/b&gt;&lt;/label&gt;
+&lt;input onkeypress='return numbers(event);'  type='input' class='form-control' id='grant_amount' name='grant_amount'  placeholder='Enter Grant Amount'/&gt;
+&lt;/div&gt;</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet12">
     <tabColor rgb="FFFF0000"/>
@@ -7989,7 +8657,7 @@
         <v>259</v>
       </c>
       <c r="F1" s="23" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="G1" s="3" t="s">
         <v>260</v>
@@ -8031,7 +8699,7 @@
         <v>271</v>
       </c>
       <c r="T1" s="38" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.45">
@@ -8159,7 +8827,489 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet13"/>
+  <dimension ref="A1:N13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="8.265625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.1328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="59.1328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.73046875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="25.86328125" bestFit="1" customWidth="1"/>
+    <col min="6" max="8" width="19.59765625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="22.73046875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="21.59765625" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="18" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="7.59765625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="9.265625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="A1" s="3" t="s">
+        <v>257</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>310</v>
+      </c>
+      <c r="D1" s="39" t="s">
+        <v>337</v>
+      </c>
+      <c r="E1" s="39" t="s">
+        <v>339</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>338</v>
+      </c>
+      <c r="G1" s="39" t="s">
+        <v>341</v>
+      </c>
+      <c r="H1" s="39" t="s">
+        <v>342</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>319</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>320</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>268</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>269</v>
+      </c>
+      <c r="M1" s="3" t="s">
+        <v>270</v>
+      </c>
+      <c r="N1" s="3" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="A2" s="3">
+        <v>1</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>309</v>
+      </c>
+      <c r="C2" s="3">
+        <v>2022</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>344</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>345</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>345</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>345</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>345</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>329</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>330</v>
+      </c>
+      <c r="K2" s="14">
+        <v>44965.416701388887</v>
+      </c>
+      <c r="L2" s="14">
+        <v>44965.416701388887</v>
+      </c>
+      <c r="M2" s="3" t="s">
+        <v>272</v>
+      </c>
+      <c r="N2" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" ht="85.5" x14ac:dyDescent="0.45">
+      <c r="D3" s="26" t="s">
+        <v>513</v>
+      </c>
+      <c r="E3" t="s">
+        <v>514</v>
+      </c>
+      <c r="G3" t="s">
+        <v>514</v>
+      </c>
+      <c r="H3" t="s">
+        <v>514</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="D4" s="76" t="s">
+        <v>343</v>
+      </c>
+      <c r="E4" s="76"/>
+      <c r="F4" s="76"/>
+      <c r="G4" s="76"/>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="C6" t="s">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="C7" s="15" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="C8" s="41" t="s">
+        <v>332</v>
+      </c>
+      <c r="D8" t="s">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="C9" s="18" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="C10" s="41" t="s">
+        <v>515</v>
+      </c>
+      <c r="D10" s="40" t="s">
+        <v>516</v>
+      </c>
+      <c r="F10" s="75" t="s">
+        <v>340</v>
+      </c>
+      <c r="G10" s="75"/>
+      <c r="H10" s="75"/>
+      <c r="I10" s="75"/>
+      <c r="J10" s="75"/>
+      <c r="K10" s="75"/>
+      <c r="L10" s="75"/>
+      <c r="M10" s="75"/>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="C11" s="18" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="C12" s="41" t="s">
+        <v>335</v>
+      </c>
+      <c r="F12" s="75" t="s">
+        <v>340</v>
+      </c>
+      <c r="G12" s="75"/>
+      <c r="H12" s="75"/>
+      <c r="I12" s="75"/>
+      <c r="J12" s="75"/>
+      <c r="K12" s="75"/>
+      <c r="L12" s="75"/>
+      <c r="M12" s="75"/>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="C13" s="41" t="s">
+        <v>336</v>
+      </c>
+      <c r="F13" s="75" t="s">
+        <v>346</v>
+      </c>
+      <c r="G13" s="75"/>
+      <c r="H13" s="75"/>
+      <c r="I13" s="75"/>
+      <c r="J13" s="75"/>
+      <c r="K13" s="75"/>
+      <c r="L13" s="75"/>
+      <c r="M13" s="75"/>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="F10:M10"/>
+    <mergeCell ref="F12:M12"/>
+    <mergeCell ref="F13:M13"/>
+    <mergeCell ref="D4:G4"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:Q24"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:Q3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="7.1328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26.86328125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.796875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.53125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.86328125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="23.59765625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.59765625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="22.33203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="17.3984375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="19.46484375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.86328125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:17" x14ac:dyDescent="0.45">
+      <c r="A1" t="s">
+        <v>257</v>
+      </c>
+      <c r="B1" t="s">
+        <v>566</v>
+      </c>
+      <c r="C1" t="s">
+        <v>567</v>
+      </c>
+      <c r="D1" t="s">
+        <v>568</v>
+      </c>
+      <c r="E1" t="s">
+        <v>569</v>
+      </c>
+      <c r="F1" t="s">
+        <v>570</v>
+      </c>
+      <c r="G1" t="s">
+        <v>571</v>
+      </c>
+      <c r="H1" t="s">
+        <v>572</v>
+      </c>
+      <c r="I1" t="s">
+        <v>573</v>
+      </c>
+      <c r="J1" t="s">
+        <v>574</v>
+      </c>
+      <c r="K1" t="s">
+        <v>575</v>
+      </c>
+      <c r="L1" t="s">
+        <v>576</v>
+      </c>
+      <c r="M1" t="s">
+        <v>577</v>
+      </c>
+      <c r="N1" s="3" t="s">
+        <v>268</v>
+      </c>
+      <c r="O1" s="3" t="s">
+        <v>269</v>
+      </c>
+      <c r="P1" s="3" t="s">
+        <v>270</v>
+      </c>
+      <c r="Q1" s="3" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.45">
+      <c r="A2" t="s">
+        <v>578</v>
+      </c>
+      <c r="B2" t="s">
+        <v>578</v>
+      </c>
+      <c r="C2" t="s">
+        <v>578</v>
+      </c>
+      <c r="D2" t="s">
+        <v>578</v>
+      </c>
+      <c r="E2" t="s">
+        <v>578</v>
+      </c>
+      <c r="F2" t="s">
+        <v>578</v>
+      </c>
+      <c r="G2" t="s">
+        <v>578</v>
+      </c>
+      <c r="H2" t="s">
+        <v>578</v>
+      </c>
+      <c r="I2" t="s">
+        <v>578</v>
+      </c>
+      <c r="J2" t="s">
+        <v>578</v>
+      </c>
+      <c r="K2" t="s">
+        <v>578</v>
+      </c>
+      <c r="L2" t="s">
+        <v>578</v>
+      </c>
+      <c r="M2" t="s">
+        <v>578</v>
+      </c>
+      <c r="N2" s="14">
+        <v>44965.416701388887</v>
+      </c>
+      <c r="O2" s="14">
+        <v>44965.416701388887</v>
+      </c>
+      <c r="P2" s="3" t="s">
+        <v>272</v>
+      </c>
+      <c r="Q2" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.45">
+      <c r="A3" t="s">
+        <v>579</v>
+      </c>
+      <c r="B3" t="s">
+        <v>579</v>
+      </c>
+      <c r="C3" t="s">
+        <v>579</v>
+      </c>
+      <c r="D3" t="s">
+        <v>579</v>
+      </c>
+      <c r="E3" t="s">
+        <v>579</v>
+      </c>
+      <c r="F3" t="s">
+        <v>579</v>
+      </c>
+      <c r="G3" t="s">
+        <v>579</v>
+      </c>
+      <c r="H3" t="s">
+        <v>579</v>
+      </c>
+      <c r="I3" t="s">
+        <v>579</v>
+      </c>
+      <c r="J3" t="s">
+        <v>579</v>
+      </c>
+      <c r="K3" t="s">
+        <v>579</v>
+      </c>
+      <c r="L3" t="s">
+        <v>579</v>
+      </c>
+      <c r="M3" t="s">
+        <v>579</v>
+      </c>
+      <c r="N3" s="14">
+        <v>44965.416701388887</v>
+      </c>
+      <c r="O3" s="14">
+        <v>44965.416701388887</v>
+      </c>
+      <c r="P3" s="3" t="s">
+        <v>272</v>
+      </c>
+      <c r="Q3" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.45">
+      <c r="K4" s="16"/>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.45">
+      <c r="K5" s="16"/>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.45">
+      <c r="A12" s="15" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.45">
+      <c r="A13" s="18" t="s">
+        <v>464</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.45">
+      <c r="A14" s="18" t="s">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.45">
+      <c r="A15" s="18" t="s">
+        <v>466</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.45">
+      <c r="A16" s="16" t="s">
+        <v>467</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A17" s="16" t="s">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A18" s="16" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A19" s="16" t="s">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A20" s="16" t="s">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A21" s="16" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A22" s="16" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A23" s="16" t="s">
+        <v>474</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A24" s="16" t="s">
+        <v>475</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet14">
     <tabColor rgb="FFFF0000"/>
@@ -8193,25 +9343,25 @@
         <v>10</v>
       </c>
       <c r="C1" s="3" t="s">
+        <v>362</v>
+      </c>
+      <c r="D1" s="3" t="s">
         <v>363</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="E1" s="3" t="s">
         <v>364</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="F1" s="3" t="s">
         <v>365</v>
       </c>
-      <c r="F1" s="3" t="s">
-        <v>366</v>
-      </c>
       <c r="G1" s="3" t="s">
+        <v>368</v>
+      </c>
+      <c r="H1" s="3" t="s">
         <v>369</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="I1" s="3" t="s">
         <v>370</v>
-      </c>
-      <c r="I1" s="3" t="s">
-        <v>371</v>
       </c>
       <c r="J1" s="3" t="s">
         <v>319</v>
@@ -8235,21 +9385,21 @@
     <row r="2" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A2" s="3"/>
       <c r="B2" s="3" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="C2" s="3"/>
       <c r="D2" s="3"/>
       <c r="E2" s="3"/>
       <c r="F2" s="9" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="G2" s="3"/>
       <c r="H2" s="3"/>
       <c r="I2" s="3" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="J2" s="3" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
       <c r="K2" s="3" t="s">
         <v>330</v>
@@ -8272,7 +9422,7 @@
         <v>1</v>
       </c>
       <c r="I3" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.45">
@@ -8280,7 +9430,7 @@
         <v>2</v>
       </c>
       <c r="I4" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.45">
@@ -8356,7 +9506,7 @@
     </row>
     <row r="15" spans="1:15" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B15" s="43" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
       <c r="D15" s="18" t="s">
         <v>356</v>
@@ -8384,7 +9534,7 @@
     </row>
     <row r="21" spans="3:7" x14ac:dyDescent="0.45">
       <c r="D21" s="7" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="E21" s="6"/>
       <c r="F21" s="6"/>
@@ -8440,489 +9590,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr codeName="Sheet13"/>
-  <dimension ref="A1:N13"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
-  <cols>
-    <col min="1" max="1" width="8.265625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.1328125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="59.1328125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.73046875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="25.86328125" bestFit="1" customWidth="1"/>
-    <col min="6" max="8" width="19.59765625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="22.73046875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="21.59765625" bestFit="1" customWidth="1"/>
-    <col min="11" max="12" width="18" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="7.59765625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="9.265625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.45">
-      <c r="A1" s="3" t="s">
-        <v>257</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>310</v>
-      </c>
-      <c r="D1" s="39" t="s">
-        <v>337</v>
-      </c>
-      <c r="E1" s="39" t="s">
-        <v>339</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>338</v>
-      </c>
-      <c r="G1" s="39" t="s">
-        <v>341</v>
-      </c>
-      <c r="H1" s="39" t="s">
-        <v>342</v>
-      </c>
-      <c r="I1" s="3" t="s">
-        <v>319</v>
-      </c>
-      <c r="J1" s="3" t="s">
-        <v>320</v>
-      </c>
-      <c r="K1" s="3" t="s">
-        <v>268</v>
-      </c>
-      <c r="L1" s="3" t="s">
-        <v>269</v>
-      </c>
-      <c r="M1" s="3" t="s">
-        <v>270</v>
-      </c>
-      <c r="N1" s="3" t="s">
-        <v>271</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.45">
-      <c r="A2" s="3">
-        <v>1</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>309</v>
-      </c>
-      <c r="C2" s="3">
-        <v>2022</v>
-      </c>
-      <c r="D2" s="5" t="s">
-        <v>344</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>345</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>345</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>345</v>
-      </c>
-      <c r="H2" s="3" t="s">
-        <v>345</v>
-      </c>
-      <c r="I2" s="3" t="s">
-        <v>329</v>
-      </c>
-      <c r="J2" s="3" t="s">
-        <v>330</v>
-      </c>
-      <c r="K2" s="14">
-        <v>44965.416701388887</v>
-      </c>
-      <c r="L2" s="14">
-        <v>44965.416701388887</v>
-      </c>
-      <c r="M2" s="3" t="s">
-        <v>272</v>
-      </c>
-      <c r="N2" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14" ht="85.5" x14ac:dyDescent="0.45">
-      <c r="D3" s="26" t="s">
-        <v>515</v>
-      </c>
-      <c r="E3" t="s">
-        <v>516</v>
-      </c>
-      <c r="G3" t="s">
-        <v>516</v>
-      </c>
-      <c r="H3" t="s">
-        <v>516</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.45">
-      <c r="D4" s="55" t="s">
-        <v>343</v>
-      </c>
-      <c r="E4" s="55"/>
-      <c r="F4" s="55"/>
-      <c r="G4" s="55"/>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.45">
-      <c r="C6" t="s">
-        <v>513</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.45">
-      <c r="C7" s="15" t="s">
-        <v>331</v>
-      </c>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.45">
-      <c r="C8" s="41" t="s">
-        <v>332</v>
-      </c>
-      <c r="D8" t="s">
-        <v>514</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.45">
-      <c r="C9" s="18" t="s">
-        <v>333</v>
-      </c>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.45">
-      <c r="C10" s="41" t="s">
-        <v>517</v>
-      </c>
-      <c r="D10" s="40" t="s">
-        <v>518</v>
-      </c>
-      <c r="F10" s="54" t="s">
-        <v>340</v>
-      </c>
-      <c r="G10" s="54"/>
-      <c r="H10" s="54"/>
-      <c r="I10" s="54"/>
-      <c r="J10" s="54"/>
-      <c r="K10" s="54"/>
-      <c r="L10" s="54"/>
-      <c r="M10" s="54"/>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.45">
-      <c r="C11" s="18" t="s">
-        <v>334</v>
-      </c>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.45">
-      <c r="C12" s="41" t="s">
-        <v>335</v>
-      </c>
-      <c r="F12" s="54" t="s">
-        <v>340</v>
-      </c>
-      <c r="G12" s="54"/>
-      <c r="H12" s="54"/>
-      <c r="I12" s="54"/>
-      <c r="J12" s="54"/>
-      <c r="K12" s="54"/>
-      <c r="L12" s="54"/>
-      <c r="M12" s="54"/>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.45">
-      <c r="C13" s="41" t="s">
-        <v>336</v>
-      </c>
-      <c r="F13" s="54" t="s">
-        <v>346</v>
-      </c>
-      <c r="G13" s="54"/>
-      <c r="H13" s="54"/>
-      <c r="I13" s="54"/>
-      <c r="J13" s="54"/>
-      <c r="K13" s="54"/>
-      <c r="L13" s="54"/>
-      <c r="M13" s="54"/>
-    </row>
-  </sheetData>
-  <mergeCells count="4">
-    <mergeCell ref="F10:M10"/>
-    <mergeCell ref="F12:M12"/>
-    <mergeCell ref="F13:M13"/>
-    <mergeCell ref="D4:G4"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q24"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:Q3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
-  <cols>
-    <col min="1" max="1" width="7.1328125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.796875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.796875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="26.86328125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.796875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.53125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.86328125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="23.59765625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16.59765625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="22.33203125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="17.3984375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="19.46484375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="13.86328125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.45">
-      <c r="A1" t="s">
-        <v>257</v>
-      </c>
-      <c r="B1" t="s">
-        <v>569</v>
-      </c>
-      <c r="C1" t="s">
-        <v>570</v>
-      </c>
-      <c r="D1" t="s">
-        <v>571</v>
-      </c>
-      <c r="E1" t="s">
-        <v>572</v>
-      </c>
-      <c r="F1" t="s">
-        <v>573</v>
-      </c>
-      <c r="G1" t="s">
-        <v>574</v>
-      </c>
-      <c r="H1" t="s">
-        <v>575</v>
-      </c>
-      <c r="I1" t="s">
-        <v>576</v>
-      </c>
-      <c r="J1" t="s">
-        <v>577</v>
-      </c>
-      <c r="K1" t="s">
-        <v>578</v>
-      </c>
-      <c r="L1" t="s">
-        <v>579</v>
-      </c>
-      <c r="M1" t="s">
-        <v>580</v>
-      </c>
-      <c r="N1" s="3" t="s">
-        <v>268</v>
-      </c>
-      <c r="O1" s="3" t="s">
-        <v>269</v>
-      </c>
-      <c r="P1" s="3" t="s">
-        <v>270</v>
-      </c>
-      <c r="Q1" s="3" t="s">
-        <v>271</v>
-      </c>
-    </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.45">
-      <c r="A2" t="s">
-        <v>581</v>
-      </c>
-      <c r="B2" t="s">
-        <v>581</v>
-      </c>
-      <c r="C2" t="s">
-        <v>581</v>
-      </c>
-      <c r="D2" t="s">
-        <v>581</v>
-      </c>
-      <c r="E2" t="s">
-        <v>581</v>
-      </c>
-      <c r="F2" t="s">
-        <v>581</v>
-      </c>
-      <c r="G2" t="s">
-        <v>581</v>
-      </c>
-      <c r="H2" t="s">
-        <v>581</v>
-      </c>
-      <c r="I2" t="s">
-        <v>581</v>
-      </c>
-      <c r="J2" t="s">
-        <v>581</v>
-      </c>
-      <c r="K2" t="s">
-        <v>581</v>
-      </c>
-      <c r="L2" t="s">
-        <v>581</v>
-      </c>
-      <c r="M2" t="s">
-        <v>581</v>
-      </c>
-      <c r="N2" s="14">
-        <v>44965.416701388887</v>
-      </c>
-      <c r="O2" s="14">
-        <v>44965.416701388887</v>
-      </c>
-      <c r="P2" s="3" t="s">
-        <v>272</v>
-      </c>
-      <c r="Q2" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.45">
-      <c r="A3" t="s">
-        <v>582</v>
-      </c>
-      <c r="B3" t="s">
-        <v>582</v>
-      </c>
-      <c r="C3" t="s">
-        <v>582</v>
-      </c>
-      <c r="D3" t="s">
-        <v>582</v>
-      </c>
-      <c r="E3" t="s">
-        <v>582</v>
-      </c>
-      <c r="F3" t="s">
-        <v>582</v>
-      </c>
-      <c r="G3" t="s">
-        <v>582</v>
-      </c>
-      <c r="H3" t="s">
-        <v>582</v>
-      </c>
-      <c r="I3" t="s">
-        <v>582</v>
-      </c>
-      <c r="J3" t="s">
-        <v>582</v>
-      </c>
-      <c r="K3" t="s">
-        <v>582</v>
-      </c>
-      <c r="L3" t="s">
-        <v>582</v>
-      </c>
-      <c r="M3" t="s">
-        <v>582</v>
-      </c>
-      <c r="N3" s="14">
-        <v>44965.416701388887</v>
-      </c>
-      <c r="O3" s="14">
-        <v>44965.416701388887</v>
-      </c>
-      <c r="P3" s="3" t="s">
-        <v>272</v>
-      </c>
-      <c r="Q3" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.45">
-      <c r="K4" s="16"/>
-    </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.45">
-      <c r="K5" s="16"/>
-    </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.45">
-      <c r="A12" s="15" t="s">
-        <v>465</v>
-      </c>
-    </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.45">
-      <c r="A13" s="18" t="s">
-        <v>466</v>
-      </c>
-    </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.45">
-      <c r="A14" s="18" t="s">
-        <v>467</v>
-      </c>
-    </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.45">
-      <c r="A15" s="18" t="s">
-        <v>468</v>
-      </c>
-    </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.45">
-      <c r="A16" s="16" t="s">
-        <v>469</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A17" s="16" t="s">
-        <v>470</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A18" s="16" t="s">
-        <v>471</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A19" s="16" t="s">
-        <v>472</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A20" s="16" t="s">
-        <v>473</v>
-      </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A21" s="16" t="s">
-        <v>474</v>
-      </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A22" s="16" t="s">
-        <v>475</v>
-      </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A23" s="16" t="s">
-        <v>476</v>
-      </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A24" s="16" t="s">
-        <v>477</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet15">
     <tabColor theme="9"/>
@@ -8943,10 +9611,10 @@
         <v>9</v>
       </c>
       <c r="B1" s="29" t="s">
+        <v>374</v>
+      </c>
+      <c r="C1" s="29" t="s">
         <v>375</v>
-      </c>
-      <c r="C1" s="29" t="s">
-        <v>376</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.45">
@@ -8954,7 +9622,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="29" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="C2" s="29">
         <v>1</v>
@@ -8965,7 +9633,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="29" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="C3" s="29">
         <v>1</v>
@@ -8976,15 +9644,15 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="9"/>
   </sheetPr>
   <dimension ref="A1:AA26"/>
   <sheetViews>
-    <sheetView topLeftCell="W1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -9010,70 +9678,70 @@
         <v>257</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>520</v>
+        <v>518</v>
       </c>
       <c r="C1" s="3" t="s">
+        <v>437</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>438</v>
+      </c>
+      <c r="E1" s="27" t="s">
         <v>439</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="F1" s="27" t="s">
+        <v>371</v>
+      </c>
+      <c r="G1" s="27" t="s">
         <v>440</v>
       </c>
-      <c r="E1" s="27" t="s">
+      <c r="H1" s="27" t="s">
         <v>441</v>
       </c>
-      <c r="F1" s="27" t="s">
-        <v>372</v>
-      </c>
-      <c r="G1" s="27" t="s">
+      <c r="I1" s="27" t="s">
         <v>442</v>
       </c>
-      <c r="H1" s="27" t="s">
-        <v>443</v>
-      </c>
-      <c r="I1" s="27" t="s">
+      <c r="J1" s="27" t="s">
+        <v>538</v>
+      </c>
+      <c r="K1" s="27" t="s">
         <v>444</v>
       </c>
-      <c r="J1" s="27" t="s">
+      <c r="L1" s="27" t="s">
+        <v>445</v>
+      </c>
+      <c r="M1" s="27" t="s">
+        <v>446</v>
+      </c>
+      <c r="N1" s="27" t="s">
+        <v>447</v>
+      </c>
+      <c r="O1" s="27" t="s">
+        <v>448</v>
+      </c>
+      <c r="P1" s="27" t="s">
+        <v>449</v>
+      </c>
+      <c r="Q1" s="27" t="s">
+        <v>450</v>
+      </c>
+      <c r="R1" s="3" t="s">
+        <v>539</v>
+      </c>
+      <c r="S1" s="3" t="s">
         <v>540</v>
       </c>
-      <c r="K1" s="27" t="s">
-        <v>446</v>
-      </c>
-      <c r="L1" s="27" t="s">
-        <v>447</v>
-      </c>
-      <c r="M1" s="27" t="s">
-        <v>448</v>
-      </c>
-      <c r="N1" s="27" t="s">
-        <v>449</v>
-      </c>
-      <c r="O1" s="27" t="s">
-        <v>450</v>
-      </c>
-      <c r="P1" s="27" t="s">
-        <v>451</v>
-      </c>
-      <c r="Q1" s="27" t="s">
-        <v>452</v>
-      </c>
-      <c r="R1" s="3" t="s">
+      <c r="T1" s="3" t="s">
         <v>541</v>
       </c>
-      <c r="S1" s="3" t="s">
-        <v>542</v>
-      </c>
-      <c r="T1" s="3" t="s">
-        <v>543</v>
-      </c>
       <c r="U1" s="3" t="s">
-        <v>560</v>
+        <v>558</v>
       </c>
       <c r="V1" s="3" t="s">
-        <v>561</v>
+        <v>559</v>
       </c>
       <c r="W1" s="3" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
       <c r="X1" s="3" t="s">
         <v>268</v>
@@ -9101,30 +9769,30 @@
       </c>
       <c r="E2" s="3"/>
       <c r="F2" s="3" t="s">
+        <v>533</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>534</v>
+      </c>
+      <c r="H2" s="3" t="s">
         <v>535</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="I2" s="3" t="s">
         <v>536</v>
       </c>
-      <c r="H2" s="3" t="s">
+      <c r="J2" s="3" t="s">
         <v>537</v>
-      </c>
-      <c r="I2" s="3" t="s">
-        <v>538</v>
-      </c>
-      <c r="J2" s="3" t="s">
-        <v>539</v>
       </c>
       <c r="K2" s="3"/>
       <c r="L2" s="3"/>
       <c r="M2" s="3"/>
       <c r="N2" s="27" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
       <c r="O2" s="3"/>
       <c r="P2" s="3"/>
       <c r="Q2" s="3" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="R2" s="3" t="s">
         <v>329</v>
@@ -9134,13 +9802,13 @@
       </c>
       <c r="T2" s="3"/>
       <c r="U2" s="3" t="s">
-        <v>565</v>
+        <v>563</v>
       </c>
       <c r="V2" s="3" t="s">
+        <v>562</v>
+      </c>
+      <c r="W2" s="3" t="s">
         <v>564</v>
-      </c>
-      <c r="W2" s="3" t="s">
-        <v>566</v>
       </c>
       <c r="X2" s="14">
         <v>44965.416701388887</v>
@@ -9157,121 +9825,121 @@
     </row>
     <row r="3" spans="1:27" x14ac:dyDescent="0.45">
       <c r="U3" s="3" t="s">
-        <v>565</v>
+        <v>563</v>
       </c>
       <c r="V3" s="3" t="s">
+        <v>562</v>
+      </c>
+      <c r="W3" s="3" t="s">
         <v>564</v>
-      </c>
-      <c r="W3" s="3" t="s">
-        <v>566</v>
       </c>
     </row>
     <row r="8" spans="1:27" x14ac:dyDescent="0.45">
       <c r="G8" s="18" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
     </row>
     <row r="9" spans="1:27" x14ac:dyDescent="0.45">
       <c r="G9" s="18" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
     </row>
     <row r="10" spans="1:27" x14ac:dyDescent="0.45">
       <c r="G10" s="18" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
     </row>
     <row r="11" spans="1:27" x14ac:dyDescent="0.45">
       <c r="G11" s="33" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
     </row>
     <row r="12" spans="1:27" x14ac:dyDescent="0.45">
       <c r="G12" s="33" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
     </row>
     <row r="13" spans="1:27" x14ac:dyDescent="0.45">
       <c r="G13" s="33" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
     </row>
     <row r="14" spans="1:27" x14ac:dyDescent="0.45">
       <c r="G14" s="18" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
     </row>
     <row r="15" spans="1:27" x14ac:dyDescent="0.45">
       <c r="G15" s="33" t="s">
-        <v>428</v>
-      </c>
-      <c r="I15" s="56" t="s">
-        <v>445</v>
+        <v>426</v>
+      </c>
+      <c r="I15" s="63" t="s">
+        <v>443</v>
       </c>
     </row>
     <row r="16" spans="1:27" x14ac:dyDescent="0.45">
       <c r="G16" s="33" t="s">
-        <v>429</v>
-      </c>
-      <c r="I16" s="56"/>
+        <v>427</v>
+      </c>
+      <c r="I16" s="63"/>
     </row>
     <row r="17" spans="7:11" x14ac:dyDescent="0.45">
       <c r="G17" s="15" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
     </row>
     <row r="18" spans="7:11" x14ac:dyDescent="0.45">
       <c r="G18" s="20" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
     </row>
     <row r="19" spans="7:11" x14ac:dyDescent="0.45">
       <c r="G19" s="18" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
     </row>
     <row r="20" spans="7:11" x14ac:dyDescent="0.45">
       <c r="G20" s="18" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
     </row>
     <row r="21" spans="7:11" x14ac:dyDescent="0.45">
       <c r="G21" s="18" t="s">
-        <v>434</v>
-      </c>
-      <c r="I21" s="57" t="s">
-        <v>454</v>
-      </c>
-      <c r="J21" s="57"/>
-      <c r="K21" s="57"/>
+        <v>432</v>
+      </c>
+      <c r="I21" s="64" t="s">
+        <v>452</v>
+      </c>
+      <c r="J21" s="64"/>
+      <c r="K21" s="64"/>
     </row>
     <row r="22" spans="7:11" x14ac:dyDescent="0.45">
       <c r="G22" s="18" t="s">
-        <v>435</v>
-      </c>
-      <c r="I22" s="57"/>
-      <c r="J22" s="57"/>
-      <c r="K22" s="57"/>
+        <v>433</v>
+      </c>
+      <c r="I22" s="64"/>
+      <c r="J22" s="64"/>
+      <c r="K22" s="64"/>
     </row>
     <row r="23" spans="7:11" x14ac:dyDescent="0.45">
       <c r="G23" s="18" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
     </row>
     <row r="24" spans="7:11" x14ac:dyDescent="0.45">
       <c r="G24" s="18" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
     </row>
     <row r="25" spans="7:11" x14ac:dyDescent="0.45">
       <c r="G25" s="18"/>
       <c r="H25" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
     </row>
     <row r="26" spans="7:11" x14ac:dyDescent="0.45">
       <c r="G26" s="34" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
     </row>
   </sheetData>
@@ -9283,15 +9951,15 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="9"/>
   </sheetPr>
   <dimension ref="A1:R18"/>
   <sheetViews>
-    <sheetView topLeftCell="I1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -9315,43 +9983,43 @@
         <v>257</v>
       </c>
       <c r="B1" s="3" t="s">
+        <v>542</v>
+      </c>
+      <c r="C1" s="48" t="s">
+        <v>543</v>
+      </c>
+      <c r="D1" s="3" t="s">
         <v>544</v>
       </c>
-      <c r="C1" s="48" t="s">
+      <c r="E1" s="3" t="s">
         <v>545</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="F1" s="3" t="s">
         <v>546</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="G1" s="3" t="s">
         <v>547</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="H1" s="3" t="s">
+        <v>540</v>
+      </c>
+      <c r="I1" s="3" t="s">
         <v>548</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="J1" s="3" t="s">
         <v>549</v>
       </c>
-      <c r="H1" s="3" t="s">
-        <v>542</v>
-      </c>
-      <c r="I1" s="3" t="s">
+      <c r="K1" s="3" t="s">
         <v>550</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="L1" s="3" t="s">
         <v>551</v>
       </c>
-      <c r="K1" s="3" t="s">
-        <v>552</v>
-      </c>
-      <c r="L1" s="3" t="s">
-        <v>553</v>
-      </c>
       <c r="M1" s="3" t="s">
-        <v>557</v>
+        <v>555</v>
       </c>
       <c r="N1" s="3" t="s">
-        <v>558</v>
+        <v>556</v>
       </c>
       <c r="O1" s="3" t="s">
         <v>268</v>
@@ -9392,13 +10060,13 @@
         <v>330</v>
       </c>
       <c r="I2" s="3" t="s">
+        <v>552</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>553</v>
+      </c>
+      <c r="K2" s="3" t="s">
         <v>554</v>
-      </c>
-      <c r="J2" s="3" t="s">
-        <v>555</v>
-      </c>
-      <c r="K2" s="3" t="s">
-        <v>556</v>
       </c>
       <c r="L2" s="3"/>
       <c r="M2" s="3"/>
@@ -9419,12 +10087,12 @@
     <row r="4" spans="1:18" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
     <row r="5" spans="1:18" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="C5" s="50" t="s">
-        <v>523</v>
+        <v>521</v>
       </c>
     </row>
     <row r="6" spans="1:18" ht="196.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="C6" s="51" t="s">
-        <v>524</v>
+        <v>522</v>
       </c>
     </row>
     <row r="7" spans="1:18" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
@@ -9432,32 +10100,32 @@
     </row>
     <row r="8" spans="1:18" ht="125.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="C8" s="52" t="s">
-        <v>525</v>
+        <v>523</v>
       </c>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.45">
       <c r="C9" s="44" t="s">
-        <v>526</v>
+        <v>524</v>
       </c>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.45">
       <c r="C10" s="44" t="s">
-        <v>527</v>
+        <v>525</v>
       </c>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.45">
       <c r="C11" s="44" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.45">
       <c r="C12" s="44" t="s">
-        <v>529</v>
+        <v>527</v>
       </c>
     </row>
     <row r="13" spans="1:18" ht="28.5" x14ac:dyDescent="0.45">
       <c r="C13" s="47" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.45">
@@ -9465,22 +10133,22 @@
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.45">
       <c r="C15" s="46" t="s">
-        <v>531</v>
+        <v>529</v>
       </c>
     </row>
     <row r="16" spans="1:18" ht="71.25" x14ac:dyDescent="0.45">
       <c r="C16" s="45" t="s">
-        <v>532</v>
+        <v>530</v>
       </c>
     </row>
     <row r="17" spans="3:3" ht="28.5" x14ac:dyDescent="0.45">
       <c r="C17" s="45" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
     </row>
     <row r="18" spans="3:3" x14ac:dyDescent="0.45">
       <c r="C18" s="46" t="s">
-        <v>534</v>
+        <v>532</v>
       </c>
     </row>
   </sheetData>
@@ -9488,7 +10156,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="5"/>
@@ -9496,7 +10164,7 @@
   <dimension ref="A1:G20"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B12" sqref="B12:E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -9510,143 +10178,143 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A1" s="58" t="s">
+      <c r="A1" s="53" t="s">
         <v>257</v>
       </c>
-      <c r="B1" s="58" t="s">
+      <c r="B1" s="53" t="s">
+        <v>557</v>
+      </c>
+      <c r="C1" s="53" t="s">
+        <v>558</v>
+      </c>
+      <c r="D1" s="53" t="s">
         <v>559</v>
       </c>
-      <c r="C1" s="58" t="s">
-        <v>560</v>
-      </c>
-      <c r="D1" s="58" t="s">
-        <v>561</v>
-      </c>
-      <c r="E1" s="58" t="s">
-        <v>482</v>
+      <c r="E1" s="53" t="s">
+        <v>480</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A2" s="3" t="s">
+        <v>560</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>561</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>563</v>
+      </c>
+      <c r="D2" s="3" t="s">
         <v>562</v>
       </c>
-      <c r="B2" s="3" t="s">
-        <v>563</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>565</v>
-      </c>
-      <c r="D2" s="3" t="s">
+      <c r="E2" s="3" t="s">
         <v>564</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>566</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A3" s="3" t="s">
-        <v>567</v>
+        <v>565</v>
       </c>
       <c r="B3" s="3" t="s">
+        <v>561</v>
+      </c>
+      <c r="C3" s="3" t="s">
         <v>563</v>
       </c>
-      <c r="C3" s="3" t="s">
-        <v>565</v>
-      </c>
       <c r="D3" s="3" t="s">
+        <v>562</v>
+      </c>
+      <c r="E3" s="3" t="s">
         <v>564</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>566</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.45">
       <c r="G7" t="s">
-        <v>521</v>
+        <v>519</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="G11" s="15" t="s">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="B12" s="65" t="s">
+        <v>580</v>
+      </c>
+      <c r="C12" s="66"/>
+      <c r="D12" s="66"/>
+      <c r="E12" s="67"/>
+      <c r="G12" s="20" t="s">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="B13" s="68"/>
+      <c r="C13" s="69"/>
+      <c r="D13" s="69"/>
+      <c r="E13" s="70"/>
+      <c r="G13" s="18" t="s">
         <v>455</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="B12" s="68" t="s">
-        <v>568</v>
-      </c>
-      <c r="C12" s="69"/>
-      <c r="D12" s="69"/>
-      <c r="E12" s="70"/>
-      <c r="G12" s="20" t="s">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="B14" s="68"/>
+      <c r="C14" s="69"/>
+      <c r="D14" s="69"/>
+      <c r="E14" s="70"/>
+      <c r="G14" s="18" t="s">
         <v>456</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="B13" s="71"/>
-      <c r="C13" s="72"/>
-      <c r="D13" s="72"/>
-      <c r="E13" s="73"/>
-      <c r="G13" s="18" t="s">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="B15" s="68"/>
+      <c r="C15" s="69"/>
+      <c r="D15" s="69"/>
+      <c r="E15" s="70"/>
+      <c r="G15" s="18" t="s">
         <v>457</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="B14" s="71"/>
-      <c r="C14" s="72"/>
-      <c r="D14" s="72"/>
-      <c r="E14" s="73"/>
-      <c r="G14" s="18" t="s">
+    <row r="16" spans="1:7" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B16" s="71"/>
+      <c r="C16" s="72"/>
+      <c r="D16" s="72"/>
+      <c r="E16" s="73"/>
+      <c r="G16" s="18" t="s">
         <v>458</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="B15" s="71"/>
-      <c r="C15" s="72"/>
-      <c r="D15" s="72"/>
-      <c r="E15" s="73"/>
-      <c r="G15" s="18" t="s">
-        <v>459</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B16" s="74"/>
-      <c r="C16" s="75"/>
-      <c r="D16" s="75"/>
-      <c r="E16" s="76"/>
-      <c r="G16" s="18" t="s">
-        <v>460</v>
       </c>
     </row>
     <row r="17" spans="2:7" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="G17" s="33" t="s">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="18" spans="2:7" x14ac:dyDescent="0.45">
+      <c r="B18" s="54"/>
+      <c r="C18" s="55"/>
+      <c r="D18" s="55"/>
+      <c r="E18" s="56"/>
+      <c r="G18" s="33" t="s">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="19" spans="2:7" x14ac:dyDescent="0.45">
+      <c r="B19" s="57"/>
+      <c r="C19" s="58"/>
+      <c r="D19" s="58"/>
+      <c r="E19" s="59"/>
+      <c r="G19" s="33" t="s">
         <v>461</v>
       </c>
     </row>
-    <row r="18" spans="2:7" x14ac:dyDescent="0.45">
-      <c r="B18" s="59"/>
-      <c r="C18" s="60"/>
-      <c r="D18" s="60"/>
-      <c r="E18" s="61"/>
-      <c r="G18" s="33" t="s">
+    <row r="20" spans="2:7" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B20" s="60"/>
+      <c r="C20" s="61"/>
+      <c r="D20" s="61"/>
+      <c r="E20" s="62"/>
+      <c r="G20" s="33" t="s">
         <v>462</v>
-      </c>
-    </row>
-    <row r="19" spans="2:7" x14ac:dyDescent="0.45">
-      <c r="B19" s="62"/>
-      <c r="C19" s="63"/>
-      <c r="D19" s="63"/>
-      <c r="E19" s="64"/>
-      <c r="G19" s="33" t="s">
-        <v>463</v>
-      </c>
-    </row>
-    <row r="20" spans="2:7" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B20" s="65"/>
-      <c r="C20" s="66"/>
-      <c r="D20" s="66"/>
-      <c r="E20" s="67"/>
-      <c r="G20" s="33" t="s">
-        <v>464</v>
       </c>
     </row>
   </sheetData>
@@ -9657,7 +10325,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="9"/>
@@ -9678,10 +10346,10 @@
         <v>9</v>
       </c>
       <c r="B1" s="36" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
       <c r="C1" s="29" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.45">
@@ -9689,7 +10357,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="37" t="s">
-        <v>481</v>
+        <v>479</v>
       </c>
       <c r="C2" s="29">
         <v>1</v>
@@ -9700,7 +10368,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="37" t="s">
-        <v>478</v>
+        <v>476</v>
       </c>
       <c r="C3" s="29">
         <v>1</v>
@@ -9711,7 +10379,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="37" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
       <c r="C4" s="29">
         <v>1</v>
@@ -9722,7 +10390,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="37" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
       <c r="C5" s="29">
         <v>1</v>
@@ -9733,7 +10401,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C17"/>
   <sheetViews>
@@ -9753,18 +10421,18 @@
         <v>9</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A2" s="3" t="s">
-        <v>483</v>
+        <v>481</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="C2" s="3">
         <v>1</v>
@@ -9772,10 +10440,10 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A3" s="3" t="s">
-        <v>484</v>
+        <v>482</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="C3" s="3">
         <v>1</v>
@@ -9783,10 +10451,10 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A4" s="3" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="C4" s="3">
         <v>1</v>
@@ -9794,10 +10462,10 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A5" s="3" t="s">
-        <v>486</v>
+        <v>484</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="C5" s="3">
         <v>1</v>
@@ -9805,10 +10473,10 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A6" s="3" t="s">
-        <v>487</v>
+        <v>485</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="C6" s="3">
         <v>1</v>
@@ -9816,10 +10484,10 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A7" s="3" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="C7" s="3">
         <v>1</v>
@@ -9827,10 +10495,10 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A8" s="3" t="s">
-        <v>489</v>
+        <v>487</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="C8" s="3">
         <v>1</v>
@@ -9838,10 +10506,10 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A9" s="3" t="s">
-        <v>490</v>
+        <v>488</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
       <c r="C9" s="3">
         <v>1</v>
@@ -9849,10 +10517,10 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A10" s="3" t="s">
-        <v>491</v>
+        <v>489</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
       <c r="C10" s="3">
         <v>1</v>
@@ -9860,10 +10528,10 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A11" s="3" t="s">
-        <v>492</v>
+        <v>490</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
       <c r="C11" s="3">
         <v>1</v>
@@ -9871,10 +10539,10 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A12" s="3" t="s">
-        <v>493</v>
+        <v>491</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>505</v>
+        <v>503</v>
       </c>
       <c r="C12" s="3">
         <v>1</v>
@@ -9882,10 +10550,10 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A13" s="3" t="s">
-        <v>494</v>
+        <v>492</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>506</v>
+        <v>504</v>
       </c>
       <c r="C13" s="3">
         <v>1</v>
@@ -9893,10 +10561,10 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A14" s="3" t="s">
-        <v>495</v>
+        <v>493</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
       <c r="C14" s="3">
         <v>1</v>
@@ -9904,10 +10572,10 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A15" s="3" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>508</v>
+        <v>506</v>
       </c>
       <c r="C15" s="3">
         <v>1</v>
@@ -9915,10 +10583,10 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A16" s="3" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
       <c r="C16" s="3">
         <v>1</v>
@@ -9926,10 +10594,10 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A17" s="3" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>510</v>
+        <v>508</v>
       </c>
       <c r="C17" s="3">
         <v>1</v>
@@ -9938,260 +10606,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr codeName="Sheet2">
-    <tabColor theme="4"/>
-  </sheetPr>
-  <dimension ref="A1:S18"/>
-  <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
-  <cols>
-    <col min="1" max="1" width="32.1328125" customWidth="1"/>
-    <col min="2" max="2" width="15" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.86328125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="22.1328125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20.73046875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.86328125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18.265625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="18.59765625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="26" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="30.3984375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="15.59765625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="17.73046875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="17.3984375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="19.73046875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="30" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="21.59765625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.45">
-      <c r="A1" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="D1" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="E1" s="9" t="s">
-        <v>231</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="H1" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="I1" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="J1" s="10" t="s">
-        <v>40</v>
-      </c>
-      <c r="K1" s="10" t="s">
-        <v>41</v>
-      </c>
-      <c r="L1" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="M1" s="9" t="s">
-        <v>232</v>
-      </c>
-      <c r="N1" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="O1" s="23" t="s">
-        <v>383</v>
-      </c>
-      <c r="P1" s="23" t="s">
-        <v>382</v>
-      </c>
-      <c r="Q1" s="23" t="s">
-        <v>384</v>
-      </c>
-      <c r="R1" s="23" t="s">
-        <v>385</v>
-      </c>
-      <c r="S1" s="24" t="s">
-        <v>414</v>
-      </c>
-    </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.45">
-      <c r="A2" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>226</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>227</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>233</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>247</v>
-      </c>
-      <c r="F2" s="5">
-        <v>44564</v>
-      </c>
-      <c r="G2" s="5">
-        <v>46111</v>
-      </c>
-      <c r="H2" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="I2" s="3" t="s">
-        <v>241</v>
-      </c>
-      <c r="J2" s="3" t="s">
-        <v>219</v>
-      </c>
-      <c r="K2" s="3" t="s">
-        <v>243</v>
-      </c>
-      <c r="L2" s="3" t="s">
-        <v>215</v>
-      </c>
-      <c r="M2" s="3" t="s">
-        <v>246</v>
-      </c>
-      <c r="N2" s="3" t="s">
-        <v>245</v>
-      </c>
-      <c r="O2" s="23" t="s">
-        <v>329</v>
-      </c>
-      <c r="P2" s="23" t="s">
-        <v>330</v>
-      </c>
-      <c r="Q2" s="23" t="s">
-        <v>329</v>
-      </c>
-      <c r="R2" s="23" t="s">
-        <v>330</v>
-      </c>
-      <c r="S2" s="24" t="s">
-        <v>387</v>
-      </c>
-    </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.45">
-      <c r="D3" t="s">
-        <v>238</v>
-      </c>
-      <c r="H3" t="s">
-        <v>239</v>
-      </c>
-      <c r="I3" t="s">
-        <v>240</v>
-      </c>
-      <c r="J3" t="s">
-        <v>242</v>
-      </c>
-      <c r="L3" t="s">
-        <v>244</v>
-      </c>
-      <c r="S3" s="25" t="s">
-        <v>388</v>
-      </c>
-    </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.45">
-      <c r="S4" s="25" t="s">
-        <v>389</v>
-      </c>
-    </row>
-    <row r="6" spans="1:19" ht="60" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B6" s="53" t="s">
-        <v>390</v>
-      </c>
-      <c r="C6" s="53"/>
-      <c r="D6" s="53"/>
-      <c r="E6" s="53"/>
-      <c r="F6" s="53"/>
-    </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.45">
-      <c r="A8" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.45">
-      <c r="A9" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.45">
-      <c r="A10" s="7" t="s">
-        <v>367</v>
-      </c>
-      <c r="B10" s="6"/>
-      <c r="C10" s="6"/>
-      <c r="D10" s="6"/>
-    </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.45">
-      <c r="A11" s="1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.45">
-      <c r="A12" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.45">
-      <c r="A13" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="B13" s="6"/>
-      <c r="C13" s="6"/>
-    </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.45">
-      <c r="A14" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="B14" s="6"/>
-      <c r="C14" s="6"/>
-    </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.45">
-      <c r="A15" s="7" t="s">
-        <v>378</v>
-      </c>
-    </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.45">
-      <c r="A16" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A17" s="7" t="s">
-        <v>43</v>
-      </c>
-      <c r="B17" s="6"/>
-      <c r="C17" s="6"/>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A18" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="C18" t="s">
-        <v>377</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="B6:F6"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
financial Reports module added
</commit_message>
<xml_diff>
--- a/web/database_design.xlsx
+++ b/web/database_design.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15210" windowHeight="6240" tabRatio="957" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15210" windowHeight="6240" tabRatio="957" firstSheet="18" activeTab="22"/>
   </bookViews>
   <sheets>
     <sheet name="key input fields" sheetId="55" r:id="rId1"/>
@@ -41,6 +41,7 @@
     <definedName name="OLE_LINK1" localSheetId="10">subrecipient_infor!$A$10</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -50,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1173" uniqueCount="683">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1281" uniqueCount="694">
   <si>
     <t>1.0 Grant Information</t>
   </si>
@@ -5339,6 +5340,39 @@
   </si>
   <si>
     <t>Options are: Fixed Amount Award/cooperative  Agreement/Contract/Assistance/Task order/Other – specify</t>
+  </si>
+  <si>
+    <t>Currently Active</t>
+  </si>
+  <si>
+    <t>Salaries</t>
+  </si>
+  <si>
+    <t>Fridge Benefits</t>
+  </si>
+  <si>
+    <t>Equipment</t>
+  </si>
+  <si>
+    <t>Travel</t>
+  </si>
+  <si>
+    <t>Supplies</t>
+  </si>
+  <si>
+    <t>Other Direct Costs</t>
+  </si>
+  <si>
+    <t>Indirect Costs</t>
+  </si>
+  <si>
+    <t>Implementation Budget</t>
+  </si>
+  <si>
+    <t>Cost Share</t>
+  </si>
+  <si>
+    <t>current_period_receipts</t>
   </si>
 </sst>
 </file>
@@ -5348,7 +5382,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy:mm:dd\ hh:mm:ss"/>
   </numFmts>
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -5422,6 +5456,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="9"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="9">
     <fill>
@@ -5473,7 +5514,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="20">
+  <borders count="27">
     <border>
       <left/>
       <right/>
@@ -5700,11 +5741,116 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="122">
+  <cellXfs count="137">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="4"/>
@@ -5902,6 +6048,58 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="22" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -5944,38 +6142,101 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="10">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -6526,8 +6787,8 @@
   </sheetPr>
   <dimension ref="A1:Q38"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+    <sheetView showGridLines="0" topLeftCell="D2" workbookViewId="0">
+      <selection activeCell="E30" sqref="E30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6729,13 +6990,13 @@
       </c>
     </row>
     <row r="6" spans="1:17" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="110" t="s">
+      <c r="B6" s="134" t="s">
         <v>386</v>
       </c>
-      <c r="C6" s="110"/>
-      <c r="D6" s="110"/>
-      <c r="E6" s="110"/>
-      <c r="F6" s="110"/>
+      <c r="C6" s="134"/>
+      <c r="D6" s="134"/>
+      <c r="E6" s="134"/>
+      <c r="F6" s="134"/>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
@@ -6814,10 +7075,10 @@
       <c r="D22" s="62" t="s">
         <v>663</v>
       </c>
-      <c r="E22" s="117" t="s">
+      <c r="E22" s="103" t="s">
         <v>587</v>
       </c>
-      <c r="F22" s="116" t="s">
+      <c r="F22" s="102" t="s">
         <v>679</v>
       </c>
     </row>
@@ -6831,7 +7092,7 @@
       <c r="D23" s="62" t="s">
         <v>664</v>
       </c>
-      <c r="E23" s="117" t="s">
+      <c r="E23" s="103" t="s">
         <v>588</v>
       </c>
       <c r="F23" s="44" t="str">
@@ -6859,11 +7120,11 @@
       <c r="D24" s="62" t="s">
         <v>665</v>
       </c>
-      <c r="E24" s="117" t="s">
+      <c r="E24" s="103" t="s">
         <v>587</v>
       </c>
       <c r="F24" s="65" t="str">
-        <f t="shared" ref="F24" si="0">"&lt;div class='form-group col-md-4'&gt;
+        <f>"&lt;div class='form-group col-md-4'&gt;
 &lt;label for='"&amp;B24&amp;"'&gt;&lt;b&gt;"&amp;D24&amp;"&lt;font color='red'&gt;*&lt;/font&gt;&lt;/b&gt;&lt;/label&gt;
 &lt;input type='input' class='form-control' id='"&amp;B24&amp;"' name='"&amp;B24&amp;"'  placeholder='Enter "&amp;D24&amp;"'/&gt;
 &lt;/div&gt;"</f>
@@ -6883,10 +7144,10 @@
       <c r="C25" s="62" t="s">
         <v>233</v>
       </c>
-      <c r="D25" s="117" t="s">
+      <c r="D25" s="103" t="s">
         <v>666</v>
       </c>
-      <c r="E25" s="117" t="s">
+      <c r="E25" s="103" t="s">
         <v>588</v>
       </c>
       <c r="F25" s="44" t="str">
@@ -6904,21 +7165,21 @@
 &lt;/div&gt;</v>
       </c>
     </row>
-    <row r="26" spans="1:6" ht="90" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" ht="105" x14ac:dyDescent="0.25">
       <c r="B26" s="80" t="s">
         <v>231</v>
       </c>
       <c r="C26" s="62" t="s">
         <v>247</v>
       </c>
-      <c r="D26" s="117" t="s">
+      <c r="D26" s="103" t="s">
         <v>667</v>
       </c>
-      <c r="E26" s="117" t="s">
+      <c r="E26" s="103" t="s">
         <v>587</v>
       </c>
       <c r="F26" s="65" t="str">
-        <f t="shared" ref="F26" si="1">"&lt;div class='form-group col-md-4'&gt;
+        <f>"&lt;div class='form-group col-md-4'&gt;
 &lt;label for='"&amp;B26&amp;"'&gt;&lt;b&gt;"&amp;D26&amp;"&lt;font color='red'&gt;*&lt;/font&gt;&lt;/b&gt;&lt;/label&gt;
 &lt;input type='input' class='form-control' id='"&amp;B26&amp;"' name='"&amp;B26&amp;"'  placeholder='Enter "&amp;D26&amp;"'/&gt;
 &lt;/div&gt;"</f>
@@ -6932,13 +7193,13 @@
       <c r="B27" s="62" t="s">
         <v>34</v>
       </c>
-      <c r="C27" s="118">
+      <c r="C27" s="104">
         <v>44564</v>
       </c>
-      <c r="D27" s="117" t="s">
+      <c r="D27" s="103" t="s">
         <v>668</v>
       </c>
-      <c r="E27" s="117" t="s">
+      <c r="E27" s="103" t="s">
         <v>610</v>
       </c>
       <c r="F27" s="65" t="str">
@@ -6956,13 +7217,13 @@
       <c r="B28" s="62" t="s">
         <v>35</v>
       </c>
-      <c r="C28" s="118">
+      <c r="C28" s="104">
         <v>46111</v>
       </c>
-      <c r="D28" s="117" t="s">
+      <c r="D28" s="103" t="s">
         <v>668</v>
       </c>
-      <c r="E28" s="117" t="s">
+      <c r="E28" s="103" t="s">
         <v>610</v>
       </c>
       <c r="F28" s="65" t="str">
@@ -6986,10 +7247,10 @@
       <c r="C29" s="62" t="s">
         <v>48</v>
       </c>
-      <c r="D29" s="117" t="s">
+      <c r="D29" s="103" t="s">
         <v>669</v>
       </c>
-      <c r="E29" s="117" t="s">
+      <c r="E29" s="103" t="s">
         <v>588</v>
       </c>
       <c r="F29" s="44" t="str">
@@ -7017,10 +7278,10 @@
       <c r="C30" s="62" t="s">
         <v>241</v>
       </c>
-      <c r="D30" s="117" t="s">
+      <c r="D30" s="103" t="s">
         <v>670</v>
       </c>
-      <c r="E30" s="117" t="s">
+      <c r="E30" s="103" t="s">
         <v>588</v>
       </c>
       <c r="F30" s="44" t="str">
@@ -7042,16 +7303,16 @@
       <c r="A31" t="s">
         <v>242</v>
       </c>
-      <c r="B31" s="119" t="s">
+      <c r="B31" s="105" t="s">
         <v>40</v>
       </c>
       <c r="C31" s="62" t="s">
         <v>219</v>
       </c>
-      <c r="D31" s="117" t="s">
+      <c r="D31" s="103" t="s">
         <v>671</v>
       </c>
-      <c r="E31" s="117" t="s">
+      <c r="E31" s="103" t="s">
         <v>588</v>
       </c>
       <c r="F31" s="44" t="str">
@@ -7076,10 +7337,10 @@
       <c r="C32" s="62" t="s">
         <v>215</v>
       </c>
-      <c r="D32" s="117" t="s">
+      <c r="D32" s="103" t="s">
         <v>673</v>
       </c>
-      <c r="E32" s="117" t="s">
+      <c r="E32" s="103" t="s">
         <v>588</v>
       </c>
       <c r="F32" s="44" t="str">
@@ -7107,14 +7368,14 @@
       <c r="C33" s="62" t="s">
         <v>246</v>
       </c>
-      <c r="D33" s="117" t="s">
+      <c r="D33" s="103" t="s">
         <v>674</v>
       </c>
-      <c r="E33" s="117" t="s">
+      <c r="E33" s="103" t="s">
         <v>587</v>
       </c>
       <c r="F33" s="65" t="str">
-        <f t="shared" ref="F33" si="2">"&lt;div class='form-group col-md-4'&gt;
+        <f>"&lt;div class='form-group col-md-4'&gt;
 &lt;label for='"&amp;B33&amp;"'&gt;&lt;b&gt;"&amp;D33&amp;"&lt;font color='red'&gt;*&lt;/font&gt;&lt;/b&gt;&lt;/label&gt;
 &lt;input type='input' class='form-control' id='"&amp;B33&amp;"' name='"&amp;B33&amp;"'  placeholder='Enter "&amp;D33&amp;"'/&gt;
 &lt;/div&gt;"</f>
@@ -7125,16 +7386,16 @@
       </c>
     </row>
     <row r="34" spans="1:6" ht="120" x14ac:dyDescent="0.25">
-      <c r="B34" s="119" t="s">
+      <c r="B34" s="105" t="s">
         <v>16</v>
       </c>
       <c r="C34" s="62" t="s">
         <v>245</v>
       </c>
-      <c r="D34" s="117" t="s">
+      <c r="D34" s="103" t="s">
         <v>583</v>
       </c>
-      <c r="E34" s="117" t="s">
+      <c r="E34" s="103" t="s">
         <v>588</v>
       </c>
       <c r="F34" s="44" t="str">
@@ -7153,16 +7414,16 @@
       </c>
     </row>
     <row r="35" spans="1:6" ht="120" x14ac:dyDescent="0.25">
-      <c r="B35" s="120" t="s">
+      <c r="B35" s="106" t="s">
         <v>380</v>
       </c>
-      <c r="C35" s="120" t="s">
+      <c r="C35" s="106" t="s">
         <v>329</v>
       </c>
-      <c r="D35" s="117" t="s">
+      <c r="D35" s="103" t="s">
         <v>675</v>
       </c>
-      <c r="E35" s="117" t="s">
+      <c r="E35" s="103" t="s">
         <v>678</v>
       </c>
       <c r="F35" s="44" t="str">
@@ -7176,17 +7437,17 @@
 &lt;/div&gt;</v>
       </c>
     </row>
-    <row r="36" spans="1:6" ht="120" x14ac:dyDescent="0.25">
-      <c r="B36" s="120" t="s">
+    <row r="36" spans="1:6" ht="105" x14ac:dyDescent="0.25">
+      <c r="B36" s="106" t="s">
         <v>381</v>
       </c>
-      <c r="C36" s="120" t="s">
+      <c r="C36" s="106" t="s">
         <v>329</v>
       </c>
       <c r="D36" s="62" t="s">
         <v>676</v>
       </c>
-      <c r="E36" s="117" t="s">
+      <c r="E36" s="103" t="s">
         <v>678</v>
       </c>
       <c r="F36" s="44" t="str">
@@ -7201,16 +7462,16 @@
       </c>
     </row>
     <row r="37" spans="1:6" ht="120" x14ac:dyDescent="0.25">
-      <c r="B37" s="121" t="s">
+      <c r="B37" s="107" t="s">
         <v>410</v>
       </c>
-      <c r="C37" s="121" t="s">
+      <c r="C37" s="107" t="s">
         <v>383</v>
       </c>
-      <c r="D37" s="120" t="s">
+      <c r="D37" s="106" t="s">
         <v>677</v>
       </c>
-      <c r="E37" s="117" t="s">
+      <c r="E37" s="103" t="s">
         <v>588</v>
       </c>
       <c r="F37" s="44" t="str">
@@ -7236,7 +7497,7 @@
     <mergeCell ref="B6:F6"/>
   </mergeCells>
   <conditionalFormatting sqref="E22:E37">
-    <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="select">
+    <cfRule type="containsText" dxfId="9" priority="1" operator="containsText" text="select">
       <formula>NOT(ISERROR(SEARCH("select",E22)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -8593,20 +8854,21 @@
   <sheetPr codeName="Sheet8">
     <tabColor theme="4"/>
   </sheetPr>
-  <dimension ref="A1:Q16"/>
+  <dimension ref="A1:Q43"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="M2" sqref="M2:N2"/>
+    <sheetView showGridLines="0" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="8.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="23.7109375" customWidth="1"/>
     <col min="5" max="5" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="42.28515625" customWidth="1"/>
+    <col min="7" max="7" width="12.140625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="17.7109375" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="13.42578125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="23.140625" bestFit="1" customWidth="1"/>
@@ -8778,7 +9040,347 @@
         <v>256</v>
       </c>
     </row>
+    <row r="19" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="20" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B20" s="108" t="s">
+        <v>257</v>
+      </c>
+      <c r="C20" s="109">
+        <v>1</v>
+      </c>
+      <c r="D20" s="110" t="s">
+        <v>663</v>
+      </c>
+      <c r="E20" s="110" t="s">
+        <v>587</v>
+      </c>
+      <c r="F20" s="111" t="s">
+        <v>679</v>
+      </c>
+    </row>
+    <row r="21" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B21" s="112" t="s">
+        <v>33</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>267</v>
+      </c>
+      <c r="D21" s="62" t="s">
+        <v>664</v>
+      </c>
+      <c r="E21" s="103" t="s">
+        <v>588</v>
+      </c>
+      <c r="F21" s="113" t="str">
+        <f>"&lt;div class='form-group col-md-4'&gt;
+&lt;label for='"&amp;B21&amp;"'&gt;&lt;b&gt;"&amp;D21&amp;"&lt;font color='red'&gt;*&lt;/font&gt;&lt;/b&gt;&lt;/label&gt;
+&lt;select required='true' class='form-control' id='"&amp;B21&amp;"' name='"&amp;B21&amp;"'  &gt;
+&lt;option value=''&gt;&lt;/option&gt;
+&lt;/select&gt;
+&lt;/div&gt;"</f>
+        <v>&lt;div class='form-group col-md-4'&gt;
+&lt;label for='subrec_id'&gt;&lt;b&gt;Sub Recipient Name&lt;font color='red'&gt;*&lt;/font&gt;&lt;/b&gt;&lt;/label&gt;
+&lt;select required='true' class='form-control' id='subrec_id' name='subrec_id'  &gt;
+&lt;option value=''&gt;&lt;/option&gt;
+&lt;/select&gt;
+&lt;/div&gt;</v>
+      </c>
+    </row>
+    <row r="22" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B22" s="112" t="s">
+        <v>258</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>281</v>
+      </c>
+      <c r="D22" s="62" t="s">
+        <v>683</v>
+      </c>
+      <c r="E22" s="103" t="s">
+        <v>588</v>
+      </c>
+      <c r="F22" s="113" t="str">
+        <f>"&lt;div class='form-group col-md-4'&gt;
+&lt;label for='"&amp;B22&amp;"'&gt;&lt;b&gt;"&amp;D22&amp;"&lt;font color='red'&gt;*&lt;/font&gt;&lt;/b&gt;&lt;/label&gt;
+&lt;select required='true' class='form-control' id='"&amp;B22&amp;"' name='"&amp;B22&amp;"'  &gt;
+&lt;option value=''&gt;&lt;/option&gt;
+&lt;/select&gt;
+&lt;/div&gt;"</f>
+        <v>&lt;div class='form-group col-md-4'&gt;
+&lt;label for='currently_active'&gt;&lt;b&gt;Currently Active&lt;font color='red'&gt;*&lt;/font&gt;&lt;/b&gt;&lt;/label&gt;
+&lt;select required='true' class='form-control' id='currently_active' name='currently_active'  &gt;
+&lt;option value=''&gt;&lt;/option&gt;
+&lt;/select&gt;
+&lt;/div&gt;</v>
+      </c>
+    </row>
+    <row r="23" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B23" s="112" t="s">
+        <v>259</v>
+      </c>
+      <c r="C23" s="3">
+        <v>100</v>
+      </c>
+      <c r="D23" s="103" t="s">
+        <v>684</v>
+      </c>
+      <c r="E23" s="103" t="s">
+        <v>587</v>
+      </c>
+      <c r="F23" s="119" t="str">
+        <f t="shared" ref="F23:F31" si="0">"&lt;div class='form-group col-md-4'&gt;
+&lt;label for='"&amp;B23&amp;"'&gt;&lt;b&gt;"&amp;D23&amp;"&lt;font color='red'&gt;*&lt;/font&gt;&lt;/b&gt;&lt;/label&gt;
+&lt;input onkeypress='return numbers(event);'  type='input' class='form-control' id='"&amp;B23&amp;"' name='"&amp;B23&amp;"'  placeholder='Enter "&amp;D23&amp;"'/&gt;
+&lt;/div&gt;"</f>
+        <v>&lt;div class='form-group col-md-4'&gt;
+&lt;label for='salaries'&gt;&lt;b&gt;Salaries&lt;font color='red'&gt;*&lt;/font&gt;&lt;/b&gt;&lt;/label&gt;
+&lt;input onkeypress='return numbers(event);'  type='input' class='form-control' id='salaries' name='salaries'  placeholder='Enter Salaries'/&gt;
+&lt;/div&gt;</v>
+      </c>
+    </row>
+    <row r="24" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B24" s="112" t="s">
+        <v>260</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>279</v>
+      </c>
+      <c r="D24" s="103" t="s">
+        <v>685</v>
+      </c>
+      <c r="E24" s="103" t="s">
+        <v>587</v>
+      </c>
+      <c r="F24" s="119" t="str">
+        <f t="shared" si="0"/>
+        <v>&lt;div class='form-group col-md-4'&gt;
+&lt;label for='fringe_benefits'&gt;&lt;b&gt;Fridge Benefits&lt;font color='red'&gt;*&lt;/font&gt;&lt;/b&gt;&lt;/label&gt;
+&lt;input onkeypress='return numbers(event);'  type='input' class='form-control' id='fringe_benefits' name='fringe_benefits'  placeholder='Enter Fridge Benefits'/&gt;
+&lt;/div&gt;</v>
+      </c>
+    </row>
+    <row r="25" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B25" s="112" t="s">
+        <v>261</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>278</v>
+      </c>
+      <c r="D25" s="103" t="s">
+        <v>686</v>
+      </c>
+      <c r="E25" s="103" t="s">
+        <v>587</v>
+      </c>
+      <c r="F25" s="119" t="str">
+        <f t="shared" si="0"/>
+        <v>&lt;div class='form-group col-md-4'&gt;
+&lt;label for='equipment'&gt;&lt;b&gt;Equipment&lt;font color='red'&gt;*&lt;/font&gt;&lt;/b&gt;&lt;/label&gt;
+&lt;input onkeypress='return numbers(event);'  type='input' class='form-control' id='equipment' name='equipment'  placeholder='Enter Equipment'/&gt;
+&lt;/div&gt;</v>
+      </c>
+    </row>
+    <row r="26" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B26" s="114" t="s">
+        <v>387</v>
+      </c>
+      <c r="C26" s="23" t="s">
+        <v>389</v>
+      </c>
+      <c r="D26" s="103" t="s">
+        <v>687</v>
+      </c>
+      <c r="E26" s="103" t="s">
+        <v>587</v>
+      </c>
+      <c r="F26" s="119" t="str">
+        <f t="shared" si="0"/>
+        <v>&lt;div class='form-group col-md-4'&gt;
+&lt;label for='travel'&gt;&lt;b&gt;Travel&lt;font color='red'&gt;*&lt;/font&gt;&lt;/b&gt;&lt;/label&gt;
+&lt;input onkeypress='return numbers(event);'  type='input' class='form-control' id='travel' name='travel'  placeholder='Enter Travel'/&gt;
+&lt;/div&gt;</v>
+      </c>
+    </row>
+    <row r="27" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B27" s="112" t="s">
+        <v>262</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>277</v>
+      </c>
+      <c r="D27" s="103" t="s">
+        <v>688</v>
+      </c>
+      <c r="E27" s="103" t="s">
+        <v>587</v>
+      </c>
+      <c r="F27" s="119" t="str">
+        <f t="shared" si="0"/>
+        <v>&lt;div class='form-group col-md-4'&gt;
+&lt;label for='supplies'&gt;&lt;b&gt;Supplies&lt;font color='red'&gt;*&lt;/font&gt;&lt;/b&gt;&lt;/label&gt;
+&lt;input onkeypress='return numbers(event);'  type='input' class='form-control' id='supplies' name='supplies'  placeholder='Enter Supplies'/&gt;
+&lt;/div&gt;</v>
+      </c>
+    </row>
+    <row r="28" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B28" s="112" t="s">
+        <v>263</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>276</v>
+      </c>
+      <c r="D28" s="103" t="s">
+        <v>689</v>
+      </c>
+      <c r="E28" s="103" t="s">
+        <v>587</v>
+      </c>
+      <c r="F28" s="119" t="str">
+        <f t="shared" si="0"/>
+        <v>&lt;div class='form-group col-md-4'&gt;
+&lt;label for='other_direct_costs'&gt;&lt;b&gt;Other Direct Costs&lt;font color='red'&gt;*&lt;/font&gt;&lt;/b&gt;&lt;/label&gt;
+&lt;input onkeypress='return numbers(event);'  type='input' class='form-control' id='other_direct_costs' name='other_direct_costs'  placeholder='Enter Other Direct Costs'/&gt;
+&lt;/div&gt;</v>
+      </c>
+    </row>
+    <row r="29" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B29" s="112" t="s">
+        <v>264</v>
+      </c>
+      <c r="C29" s="3" t="s">
+        <v>275</v>
+      </c>
+      <c r="D29" s="103" t="s">
+        <v>690</v>
+      </c>
+      <c r="E29" s="103" t="s">
+        <v>587</v>
+      </c>
+      <c r="F29" s="119" t="str">
+        <f t="shared" si="0"/>
+        <v>&lt;div class='form-group col-md-4'&gt;
+&lt;label for='indirect_costs'&gt;&lt;b&gt;Indirect Costs&lt;font color='red'&gt;*&lt;/font&gt;&lt;/b&gt;&lt;/label&gt;
+&lt;input onkeypress='return numbers(event);'  type='input' class='form-control' id='indirect_costs' name='indirect_costs'  placeholder='Enter Indirect Costs'/&gt;
+&lt;/div&gt;</v>
+      </c>
+    </row>
+    <row r="30" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B30" s="112" t="s">
+        <v>265</v>
+      </c>
+      <c r="C30" s="3" t="s">
+        <v>274</v>
+      </c>
+      <c r="D30" s="103" t="s">
+        <v>691</v>
+      </c>
+      <c r="E30" s="103" t="s">
+        <v>587</v>
+      </c>
+      <c r="F30" s="119" t="str">
+        <f t="shared" si="0"/>
+        <v>&lt;div class='form-group col-md-4'&gt;
+&lt;label for='implementation_budget'&gt;&lt;b&gt;Implementation Budget&lt;font color='red'&gt;*&lt;/font&gt;&lt;/b&gt;&lt;/label&gt;
+&lt;input onkeypress='return numbers(event);'  type='input' class='form-control' id='implementation_budget' name='implementation_budget'  placeholder='Enter Implementation Budget'/&gt;
+&lt;/div&gt;</v>
+      </c>
+    </row>
+    <row r="31" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B31" s="112" t="s">
+        <v>266</v>
+      </c>
+      <c r="C31" s="3" t="s">
+        <v>273</v>
+      </c>
+      <c r="D31" s="103" t="s">
+        <v>692</v>
+      </c>
+      <c r="E31" s="103" t="s">
+        <v>587</v>
+      </c>
+      <c r="F31" s="119" t="str">
+        <f t="shared" si="0"/>
+        <v>&lt;div class='form-group col-md-4'&gt;
+&lt;label for='cost_share'&gt;&lt;b&gt;Cost Share&lt;font color='red'&gt;*&lt;/font&gt;&lt;/b&gt;&lt;/label&gt;
+&lt;input onkeypress='return numbers(event);'  type='input' class='form-control' id='cost_share' name='cost_share'  placeholder='Enter Cost Share'/&gt;
+&lt;/div&gt;</v>
+      </c>
+    </row>
+    <row r="32" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B32" s="115" t="s">
+        <v>402</v>
+      </c>
+      <c r="C32" s="116" t="s">
+        <v>401</v>
+      </c>
+      <c r="D32" s="117"/>
+      <c r="E32" s="117" t="s">
+        <v>588</v>
+      </c>
+      <c r="F32" s="118" t="str">
+        <f>"&lt;div class='form-group col-md-4'&gt;
+&lt;label for='"&amp;B32&amp;"'&gt;&lt;b&gt;"&amp;D32&amp;"&lt;font color='red'&gt;*&lt;/font&gt;&lt;/b&gt;&lt;/label&gt;
+&lt;select required='true' class='form-control' id='"&amp;B32&amp;"' name='"&amp;B32&amp;"'  &gt;
+&lt;option value=''&gt;&lt;/option&gt;
+&lt;/select&gt;
+&lt;/div&gt;"</f>
+        <v>&lt;div class='form-group col-md-4'&gt;
+&lt;label for='update_no'&gt;&lt;b&gt;&lt;font color='red'&gt;*&lt;/font&gt;&lt;/b&gt;&lt;/label&gt;
+&lt;select required='true' class='form-control' id='update_no' name='update_no'  &gt;
+&lt;option value=''&gt;&lt;/option&gt;
+&lt;/select&gt;
+&lt;/div&gt;</v>
+      </c>
+    </row>
+    <row r="43" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F43" s="120"/>
+    </row>
   </sheetData>
+  <conditionalFormatting sqref="E20:E21 E24 E31:E32">
+    <cfRule type="containsText" dxfId="8" priority="9" operator="containsText" text="select">
+      <formula>NOT(ISERROR(SEARCH("select",E20)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E22">
+    <cfRule type="containsText" dxfId="7" priority="8" operator="containsText" text="select">
+      <formula>NOT(ISERROR(SEARCH("select",E22)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E23">
+    <cfRule type="containsText" dxfId="6" priority="7" operator="containsText" text="select">
+      <formula>NOT(ISERROR(SEARCH("select",E23)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E25">
+    <cfRule type="containsText" dxfId="5" priority="6" operator="containsText" text="select">
+      <formula>NOT(ISERROR(SEARCH("select",E25)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E26">
+    <cfRule type="containsText" dxfId="4" priority="5" operator="containsText" text="select">
+      <formula>NOT(ISERROR(SEARCH("select",E26)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E27">
+    <cfRule type="containsText" dxfId="3" priority="4" operator="containsText" text="select">
+      <formula>NOT(ISERROR(SEARCH("select",E27)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E28">
+    <cfRule type="containsText" dxfId="2" priority="3" operator="containsText" text="select">
+      <formula>NOT(ISERROR(SEARCH("select",E28)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E29">
+    <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="select">
+      <formula>NOT(ISERROR(SEARCH("select",E29)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E30">
+    <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="select">
+      <formula>NOT(ISERROR(SEARCH("select",E30)))</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -8791,7 +9393,7 @@
   <dimension ref="A1:R18"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8992,7 +9594,7 @@
   </sheetPr>
   <dimension ref="A1:K33"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A26" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="A26" workbookViewId="0">
       <selection activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
@@ -9412,12 +10014,12 @@
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet10">
-    <tabColor theme="4"/>
+    <tabColor theme="5"/>
   </sheetPr>
-  <dimension ref="A1:AK19"/>
+  <dimension ref="A1:AK37"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="C23" sqref="C22:C23"/>
+    <sheetView showGridLines="0" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9425,11 +10027,11 @@
     <col min="1" max="1" width="8.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="36.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="62.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="30" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="76" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="61" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="32.42578125" customWidth="1"/>
+    <col min="5" max="5" width="22.42578125" customWidth="1"/>
+    <col min="6" max="6" width="19.140625" customWidth="1"/>
+    <col min="7" max="7" width="30.140625" customWidth="1"/>
+    <col min="8" max="8" width="32.85546875" customWidth="1"/>
     <col min="9" max="9" width="25.85546875" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="33.28515625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="34.140625" bestFit="1" customWidth="1"/>
@@ -9698,19 +10300,155 @@
         <v>393</v>
       </c>
     </row>
-    <row r="17" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="3:7" x14ac:dyDescent="0.25">
       <c r="G17" s="23" t="s">
         <v>394</v>
       </c>
     </row>
-    <row r="18" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="3:7" x14ac:dyDescent="0.25">
       <c r="G18" s="23" t="s">
         <v>395</v>
       </c>
     </row>
-    <row r="19" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="3:7" x14ac:dyDescent="0.25">
       <c r="G19" s="23" t="s">
         <v>396</v>
+      </c>
+    </row>
+    <row r="21" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C21" s="29" t="s">
+        <v>257</v>
+      </c>
+      <c r="D21" s="29" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="22" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C22" s="29" t="s">
+        <v>33</v>
+      </c>
+      <c r="D22" s="29" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="23" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C23" s="29" t="s">
+        <v>397</v>
+      </c>
+      <c r="D23" s="32" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="24" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C24" s="29" t="s">
+        <v>302</v>
+      </c>
+      <c r="D24" s="29" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="25" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C25" s="29" t="s">
+        <v>303</v>
+      </c>
+      <c r="D25" s="31" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="26" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C26" s="29" t="s">
+        <v>304</v>
+      </c>
+      <c r="D26" s="29" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="27" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C27" s="29" t="s">
+        <v>295</v>
+      </c>
+      <c r="D27" s="29" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="28" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C28" s="29" t="s">
+        <v>305</v>
+      </c>
+      <c r="D28" s="29" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="29" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C29" s="30" t="s">
+        <v>390</v>
+      </c>
+      <c r="D29" s="29" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="30" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C30" s="30" t="s">
+        <v>391</v>
+      </c>
+      <c r="D30" s="29" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="31" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C31" s="30" t="s">
+        <v>392</v>
+      </c>
+      <c r="D31" s="29" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="32" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C32" s="30" t="s">
+        <v>393</v>
+      </c>
+      <c r="D32" s="29" t="s">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="33" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C33" s="30" t="s">
+        <v>394</v>
+      </c>
+      <c r="D33" s="29" t="s">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="34" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C34" s="30" t="s">
+        <v>395</v>
+      </c>
+      <c r="D34" s="29" t="s">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="35" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C35" s="30" t="s">
+        <v>396</v>
+      </c>
+      <c r="D35" s="29" t="s">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="36" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C36" s="31" t="s">
+        <v>399</v>
+      </c>
+      <c r="D36" s="29" t="s">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="37" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C37" s="31" t="s">
+        <v>400</v>
+      </c>
+      <c r="D37" s="29" t="s">
+        <v>415</v>
       </c>
     </row>
   </sheetData>
@@ -9722,12 +10460,12 @@
 <file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet12">
-    <tabColor rgb="FFFF0000"/>
+    <tabColor theme="8"/>
   </sheetPr>
-  <dimension ref="A1:T19"/>
+  <dimension ref="A1:T43"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="L1" workbookViewId="0">
-      <selection activeCell="N1" sqref="N1"/>
+    <sheetView showGridLines="0" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="E44" sqref="E44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9735,7 +10473,7 @@
     <col min="1" max="1" width="8.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="53.42578125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="14.85546875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="10.85546875" bestFit="1" customWidth="1"/>
@@ -9917,19 +10655,129 @@
         <v>253</v>
       </c>
     </row>
-    <row r="17" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="4:5" x14ac:dyDescent="0.25">
       <c r="E17" s="13" t="s">
         <v>254</v>
       </c>
     </row>
-    <row r="18" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="4:5" x14ac:dyDescent="0.25">
       <c r="E18" s="13" t="s">
         <v>315</v>
       </c>
     </row>
-    <row r="19" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="4:5" x14ac:dyDescent="0.25">
       <c r="E19" s="19" t="s">
         <v>316</v>
+      </c>
+    </row>
+    <row r="30" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D30" s="3" t="s">
+        <v>310</v>
+      </c>
+      <c r="E30" s="3">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="31" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D31" s="3" t="s">
+        <v>317</v>
+      </c>
+      <c r="E31" s="5">
+        <v>44965</v>
+      </c>
+    </row>
+    <row r="32" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D32" s="122" t="s">
+        <v>259</v>
+      </c>
+      <c r="E32" s="3" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="33" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D33" s="121" t="s">
+        <v>387</v>
+      </c>
+      <c r="E33" s="23"/>
+    </row>
+    <row r="34" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D34" s="122" t="s">
+        <v>260</v>
+      </c>
+      <c r="E34" s="3" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="35" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D35" s="122" t="s">
+        <v>261</v>
+      </c>
+      <c r="E35" s="3" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="36" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D36" s="122" t="s">
+        <v>262</v>
+      </c>
+      <c r="E36" s="3" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="37" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D37" s="122" t="s">
+        <v>263</v>
+      </c>
+      <c r="E37" s="3" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="38" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D38" s="122" t="s">
+        <v>264</v>
+      </c>
+      <c r="E38" s="3" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="39" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D39" s="122" t="s">
+        <v>318</v>
+      </c>
+      <c r="E39" s="3" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="40" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D40" s="122" t="s">
+        <v>266</v>
+      </c>
+      <c r="E40" s="3" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="41" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D41" s="3" t="s">
+        <v>319</v>
+      </c>
+      <c r="E41" s="3" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="42" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D42" s="3" t="s">
+        <v>320</v>
+      </c>
+      <c r="E42" s="3" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="43" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D43" s="37" t="s">
+        <v>693</v>
+      </c>
+      <c r="E43" s="37">
+        <v>7873468837</v>
       </c>
     </row>
   </sheetData>
@@ -9939,11 +10787,13 @@
 
 <file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr codeName="Sheet13"/>
+  <sheetPr codeName="Sheet13">
+    <tabColor theme="5"/>
+  </sheetPr>
   <dimension ref="A1:N13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10064,12 +10914,12 @@
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="D4" s="112" t="s">
+      <c r="D4" s="136" t="s">
         <v>343</v>
       </c>
-      <c r="E4" s="112"/>
-      <c r="F4" s="112"/>
-      <c r="G4" s="112"/>
+      <c r="E4" s="136"/>
+      <c r="F4" s="136"/>
+      <c r="G4" s="136"/>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="C6" t="s">
@@ -10101,16 +10951,16 @@
       <c r="D10" s="39" t="s">
         <v>514</v>
       </c>
-      <c r="F10" s="111" t="s">
+      <c r="F10" s="135" t="s">
         <v>340</v>
       </c>
-      <c r="G10" s="111"/>
-      <c r="H10" s="111"/>
-      <c r="I10" s="111"/>
-      <c r="J10" s="111"/>
-      <c r="K10" s="111"/>
-      <c r="L10" s="111"/>
-      <c r="M10" s="111"/>
+      <c r="G10" s="135"/>
+      <c r="H10" s="135"/>
+      <c r="I10" s="135"/>
+      <c r="J10" s="135"/>
+      <c r="K10" s="135"/>
+      <c r="L10" s="135"/>
+      <c r="M10" s="135"/>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="C11" s="18" t="s">
@@ -10121,31 +10971,31 @@
       <c r="C12" s="40" t="s">
         <v>335</v>
       </c>
-      <c r="F12" s="111" t="s">
+      <c r="F12" s="135" t="s">
         <v>340</v>
       </c>
-      <c r="G12" s="111"/>
-      <c r="H12" s="111"/>
-      <c r="I12" s="111"/>
-      <c r="J12" s="111"/>
-      <c r="K12" s="111"/>
-      <c r="L12" s="111"/>
-      <c r="M12" s="111"/>
+      <c r="G12" s="135"/>
+      <c r="H12" s="135"/>
+      <c r="I12" s="135"/>
+      <c r="J12" s="135"/>
+      <c r="K12" s="135"/>
+      <c r="L12" s="135"/>
+      <c r="M12" s="135"/>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="C13" s="40" t="s">
         <v>336</v>
       </c>
-      <c r="F13" s="111" t="s">
+      <c r="F13" s="135" t="s">
         <v>346</v>
       </c>
-      <c r="G13" s="111"/>
-      <c r="H13" s="111"/>
-      <c r="I13" s="111"/>
-      <c r="J13" s="111"/>
-      <c r="K13" s="111"/>
-      <c r="L13" s="111"/>
-      <c r="M13" s="111"/>
+      <c r="G13" s="135"/>
+      <c r="H13" s="135"/>
+      <c r="I13" s="135"/>
+      <c r="J13" s="135"/>
+      <c r="K13" s="135"/>
+      <c r="L13" s="135"/>
+      <c r="M13" s="135"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -10161,15 +11011,18 @@
 
 <file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor theme="5"/>
+  </sheetPr>
   <dimension ref="A1:Q24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:Q3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="113.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="26.85546875" bestFit="1" customWidth="1"/>
@@ -10426,8 +11279,8 @@
   </sheetPr>
   <dimension ref="A1:O44"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="E36" sqref="E36"/>
+    <sheetView showGridLines="0" topLeftCell="B36" workbookViewId="0">
+      <selection activeCell="F38" sqref="F38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10759,7 +11612,7 @@
         <v>588</v>
       </c>
       <c r="E35" s="65" t="str">
-        <f t="shared" ref="E35" si="0">"&lt;div class='form-group col-md-4'&gt;
+        <f>"&lt;div class='form-group col-md-4'&gt;
 &lt;label for='"&amp;A35&amp;"'&gt;&lt;b&gt;"&amp;C35&amp;"&lt;font color='red'&gt;*&lt;/font&gt;&lt;/b&gt;&lt;/label&gt;
 &lt;input type='input' class='form-control' id='"&amp;A35&amp;"' name='"&amp;A35&amp;"'  placeholder='Enter "&amp;C35&amp;"'/&gt;
 &lt;/div&gt;"</f>
@@ -10781,7 +11634,7 @@
         <v>587</v>
       </c>
       <c r="E36" s="65" t="str">
-        <f t="shared" ref="E36" si="1">"&lt;div class='form-group col-md-4'&gt;
+        <f>"&lt;div class='form-group col-md-4'&gt;
 &lt;label for='"&amp;A36&amp;"'&gt;&lt;b&gt;"&amp;C36&amp;"&lt;font color='red'&gt;*&lt;/font&gt;&lt;/b&gt;&lt;/label&gt;
 &lt;input type='input' class='form-control' id='"&amp;A36&amp;"' name='"&amp;A36&amp;"'  placeholder='Enter "&amp;C36&amp;"'/&gt;
 &lt;/div&gt;"</f>
@@ -10907,7 +11760,7 @@
         <v>588</v>
       </c>
       <c r="E42" s="65" t="str">
-        <f t="shared" ref="E42:E43" si="2">"&lt;div class='form-group col-md-4'&gt;
+        <f>"&lt;div class='form-group col-md-4'&gt;
 &lt;label for='"&amp;A42&amp;"'&gt;&lt;b&gt;"&amp;C42&amp;"&lt;font color='red'&gt;*&lt;/font&gt;&lt;/b&gt;&lt;/label&gt;
 &lt;input type='input' class='form-control' id='"&amp;A42&amp;"' name='"&amp;A42&amp;"'  placeholder='Enter "&amp;C42&amp;"'/&gt;
 &lt;/div&gt;"</f>
@@ -10931,7 +11784,10 @@
         <v>587</v>
       </c>
       <c r="E43" s="65" t="str">
-        <f t="shared" si="2"/>
+        <f>"&lt;div class='form-group col-md-4'&gt;
+&lt;label for='"&amp;A43&amp;"'&gt;&lt;b&gt;"&amp;C43&amp;"&lt;font color='red'&gt;*&lt;/font&gt;&lt;/b&gt;&lt;/label&gt;
+&lt;input type='input' class='form-control' id='"&amp;A43&amp;"' name='"&amp;A43&amp;"'  placeholder='Enter "&amp;C43&amp;"'/&gt;
+&lt;/div&gt;"</f>
         <v>&lt;div class='form-group col-md-4'&gt;
 &lt;label for='attachment_name'&gt;&lt;b&gt;Documents Name(s)&lt;font color='red'&gt;*&lt;/font&gt;&lt;/b&gt;&lt;/label&gt;
 &lt;input type='input' class='form-control' id='attachment_name' name='attachment_name'  placeholder='Enter Documents Name(s)'/&gt;
@@ -11439,7 +12295,7 @@
       <c r="G15" s="2" t="s">
         <v>424</v>
       </c>
-      <c r="I15" s="99" t="s">
+      <c r="I15" s="123" t="s">
         <v>441</v>
       </c>
     </row>
@@ -11469,7 +12325,7 @@
       <c r="G16" s="2" t="s">
         <v>425</v>
       </c>
-      <c r="I16" s="99"/>
+      <c r="I16" s="123"/>
     </row>
     <row r="17" spans="2:11" s="15" customFormat="1" ht="105" x14ac:dyDescent="0.25">
       <c r="B17" s="84" t="s">
@@ -11629,11 +12485,11 @@
       <c r="G21" s="85" t="s">
         <v>430</v>
       </c>
-      <c r="I21" s="100" t="s">
+      <c r="I21" s="124" t="s">
         <v>450</v>
       </c>
-      <c r="J21" s="100"/>
-      <c r="K21" s="100"/>
+      <c r="J21" s="124"/>
+      <c r="K21" s="124"/>
     </row>
     <row r="22" spans="2:11" s="15" customFormat="1" ht="105" x14ac:dyDescent="0.25">
       <c r="B22" s="84" t="s">
@@ -11659,9 +12515,9 @@
       <c r="G22" s="85" t="s">
         <v>431</v>
       </c>
-      <c r="I22" s="100"/>
-      <c r="J22" s="100"/>
-      <c r="K22" s="100"/>
+      <c r="I22" s="124"/>
+      <c r="J22" s="124"/>
+      <c r="K22" s="124"/>
     </row>
     <row r="23" spans="2:11" s="15" customFormat="1" ht="150" x14ac:dyDescent="0.25">
       <c r="B23" s="81" t="s">
@@ -11967,7 +12823,7 @@
   </sheetPr>
   <dimension ref="A1:Q35"/>
   <sheetViews>
-    <sheetView topLeftCell="A26" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView topLeftCell="A23" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
@@ -12191,7 +13047,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="16" spans="1:17" ht="180" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="C16"/>
       <c r="E16" s="44" t="s">
         <v>528</v>
@@ -12391,7 +13247,7 @@
         <v>587</v>
       </c>
       <c r="E31" s="44" t="str">
-        <f t="shared" ref="E31:E33" si="0">"&lt;div class='form-group col-md-4'&gt;
+        <f>"&lt;div class='form-group col-md-4'&gt;
 &lt;label for='"&amp;A31&amp;"'&gt;&lt;b&gt;"&amp;C31&amp;"&lt;font color='red'&gt;*&lt;/font&gt;&lt;/b&gt;&lt;/label&gt;
 &lt;input required='true' type='file' class='form-control' id='"&amp;A31&amp;"' name='"&amp;A31&amp;"'  placeholder='Enter "&amp;C31&amp;"'/&gt;
 &lt;/div&gt;"</f>
@@ -12413,7 +13269,10 @@
         <v>587</v>
       </c>
       <c r="E32" s="44" t="str">
-        <f t="shared" si="0"/>
+        <f>"&lt;div class='form-group col-md-4'&gt;
+&lt;label for='"&amp;A32&amp;"'&gt;&lt;b&gt;"&amp;C32&amp;"&lt;font color='red'&gt;*&lt;/font&gt;&lt;/b&gt;&lt;/label&gt;
+&lt;input required='true' type='file' class='form-control' id='"&amp;A32&amp;"' name='"&amp;A32&amp;"'  placeholder='Enter "&amp;C32&amp;"'/&gt;
+&lt;/div&gt;"</f>
         <v>&lt;div class='form-group col-md-4'&gt;
 &lt;label for='finance_evaluation_attachment'&gt;&lt;b&gt;Finance Evaluation attachment&lt;font color='red'&gt;*&lt;/font&gt;&lt;/b&gt;&lt;/label&gt;
 &lt;input required='true' type='file' class='form-control' id='finance_evaluation_attachment' name='finance_evaluation_attachment'  placeholder='Enter Finance Evaluation attachment'/&gt;
@@ -12432,7 +13291,10 @@
         <v>587</v>
       </c>
       <c r="E33" s="44" t="str">
-        <f t="shared" si="0"/>
+        <f>"&lt;div class='form-group col-md-4'&gt;
+&lt;label for='"&amp;A33&amp;"'&gt;&lt;b&gt;"&amp;C33&amp;"&lt;font color='red'&gt;*&lt;/font&gt;&lt;/b&gt;&lt;/label&gt;
+&lt;input required='true' type='file' class='form-control' id='"&amp;A33&amp;"' name='"&amp;A33&amp;"'  placeholder='Enter "&amp;C33&amp;"'/&gt;
+&lt;/div&gt;"</f>
         <v>&lt;div class='form-group col-md-4'&gt;
 &lt;label for='other_evaluation_attachment'&gt;&lt;b&gt;Other Evaluation Attachments&lt;font color='red'&gt;*&lt;/font&gt;&lt;/b&gt;&lt;/label&gt;
 &lt;input required='true' type='file' class='form-control' id='other_evaluation_attachment' name='other_evaluation_attachment'  placeholder='Enter Other Evaluation Attachments'/&gt;
@@ -12503,8 +13365,8 @@
   </sheetPr>
   <dimension ref="A1:G31"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="F30" sqref="F30"/>
+    <sheetView showGridLines="0" topLeftCell="A29" workbookViewId="0">
+      <selection activeCell="F29" sqref="F29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12597,48 +13459,48 @@
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B12" s="101" t="s">
+      <c r="B12" s="125" t="s">
         <v>574</v>
       </c>
-      <c r="C12" s="102"/>
-      <c r="D12" s="102"/>
-      <c r="E12" s="103"/>
+      <c r="C12" s="126"/>
+      <c r="D12" s="126"/>
+      <c r="E12" s="127"/>
       <c r="G12" s="20" t="s">
         <v>452</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B13" s="104"/>
-      <c r="C13" s="105"/>
-      <c r="D13" s="105"/>
-      <c r="E13" s="106"/>
+      <c r="B13" s="128"/>
+      <c r="C13" s="129"/>
+      <c r="D13" s="129"/>
+      <c r="E13" s="130"/>
       <c r="G13" s="18" t="s">
         <v>453</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B14" s="104"/>
-      <c r="C14" s="105"/>
-      <c r="D14" s="105"/>
-      <c r="E14" s="106"/>
+      <c r="B14" s="128"/>
+      <c r="C14" s="129"/>
+      <c r="D14" s="129"/>
+      <c r="E14" s="130"/>
       <c r="G14" s="18" t="s">
         <v>454</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B15" s="104"/>
-      <c r="C15" s="105"/>
-      <c r="D15" s="105"/>
-      <c r="E15" s="106"/>
+      <c r="B15" s="128"/>
+      <c r="C15" s="129"/>
+      <c r="D15" s="129"/>
+      <c r="E15" s="130"/>
       <c r="G15" s="18" t="s">
         <v>455</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="107"/>
-      <c r="C16" s="108"/>
-      <c r="D16" s="108"/>
-      <c r="E16" s="109"/>
+      <c r="B16" s="131"/>
+      <c r="C16" s="132"/>
+      <c r="D16" s="132"/>
+      <c r="E16" s="133"/>
       <c r="G16" s="18" t="s">
         <v>456</v>
       </c>
@@ -12683,10 +13545,10 @@
       <c r="D26" s="92" t="s">
         <v>609</v>
       </c>
-      <c r="E26" s="114" t="s">
+      <c r="E26" s="100" t="s">
         <v>586</v>
       </c>
-      <c r="F26" s="114" t="s">
+      <c r="F26" s="100" t="s">
         <v>586</v>
       </c>
     </row>
@@ -12718,7 +13580,7 @@
 &lt;/div&gt;</v>
       </c>
     </row>
-    <row r="28" spans="2:7" s="48" customFormat="1" ht="120" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:7" s="48" customFormat="1" ht="105" x14ac:dyDescent="0.25">
       <c r="B28" s="52" t="s">
         <v>435</v>
       </c>
@@ -12731,7 +13593,7 @@
       <c r="E28" s="4" t="s">
         <v>587</v>
       </c>
-      <c r="F28" s="113" t="str">
+      <c r="F28" s="99" t="str">
         <f>"&lt;div class='form-group col-md-4'&gt;
 &lt;label for='"&amp;B28&amp;"'&gt;&lt;b&gt;"&amp;D28&amp;"&lt;font color='red'&gt;*&lt;/font&gt;&lt;/b&gt;&lt;/label&gt;
 &lt;input onkeypress='return numbers(event);'  type='input' class='form-control' id='"&amp;B28&amp;"' name='"&amp;B28&amp;"'  placeholder='Enter "&amp;D28&amp;"'/&gt;
@@ -12752,10 +13614,10 @@
       <c r="D29" s="3" t="s">
         <v>660</v>
       </c>
-      <c r="E29" s="115" t="s">
+      <c r="E29" s="101" t="s">
         <v>587</v>
       </c>
-      <c r="F29" s="113" t="str">
+      <c r="F29" s="99" t="str">
         <f>"&lt;div class='form-group col-md-4'&gt;
 &lt;label for='"&amp;B29&amp;"'&gt;&lt;b&gt;"&amp;D29&amp;"&lt;font color='red'&gt;*&lt;/font&gt;&lt;/b&gt;&lt;/label&gt;
 &lt;input onkeypress='return numbers(event);'  type='input' class='form-control' id='"&amp;B29&amp;"' name='"&amp;B29&amp;"'  placeholder='Enter "&amp;D29&amp;"'/&gt;

</xml_diff>